<commit_message>
MF file updated file uploaded
</commit_message>
<xml_diff>
--- a/MF-Tracker-online.xlsx
+++ b/MF-Tracker-online.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13035"/>
+    <workbookView windowWidth="24300" windowHeight="13035"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28">
   <si>
     <t>Company Name</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>Reliance Large Cap Fund - Direct Plan (G)</t>
+  </si>
+  <si>
+    <t>https://www.valueresearchonline.com/funds/newsnapshot.asp?schemecode=16192</t>
   </si>
   <si>
     <t>Canara Robeco Emerging Equities - Direct Plan (G)</t>
@@ -105,14 +108,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="9">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="[$-409]d/mmm/yy"/>
     <numFmt numFmtId="180" formatCode="d&quot;-&quot;mmm&quot;-&quot;yyyy"/>
-    <numFmt numFmtId="181" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="182" formatCode="0.000"/>
-    <numFmt numFmtId="183" formatCode="0.0"/>
+    <numFmt numFmtId="181" formatCode="0.0"/>
+    <numFmt numFmtId="182" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="183" formatCode="0.000"/>
     <numFmt numFmtId="184" formatCode="0.000_ "/>
   </numFmts>
   <fonts count="28">
@@ -185,7 +188,36 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -193,6 +225,30 @@
     <font>
       <b/>
       <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -207,11 +263,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -232,58 +294,6 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -298,14 +308,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -313,8 +315,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -359,7 +362,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -371,139 +524,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -519,32 +546,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="20">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -683,11 +686,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color auto="1"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -697,15 +713,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -740,32 +747,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -784,18 +765,26 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -804,136 +793,139 @@
     <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="182" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -973,10 +965,10 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1002,11 +994,11 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1039,11 +1031,11 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1054,21 +1046,21 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="183" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1078,7 +1070,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1093,10 +1085,6 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1104,11 +1092,11 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="183" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="183" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1132,7 +1120,7 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1186,6 +1174,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1540,15 +1529,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H1217"/>
+  <dimension ref="A1:I1222"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A266" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="K74" sqref="K74"/>
+      <selection pane="bottomLeft" activeCell="G286" sqref="G286"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="47.2857142857143" customWidth="1"/>
     <col min="2" max="2" width="20.5714285714286" style="17" customWidth="1"/>
@@ -1558,7 +1547,8 @@
     <col min="6" max="6" width="14.8571428571429" customWidth="1"/>
     <col min="7" max="7" width="12.4285714285714" customWidth="1"/>
     <col min="8" max="8" width="13.2857142857143" customWidth="1"/>
-    <col min="9" max="26" width="8.71428571428571" customWidth="1"/>
+    <col min="9" max="9" width="85.5714285714286" customWidth="1"/>
+    <col min="10" max="26" width="8.71428571428571" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.75" customHeight="1" spans="1:8">
@@ -2311,22 +2301,42 @@
     <row r="35" ht="24.75" customHeight="1" spans="1:8">
       <c r="A35" s="25"/>
       <c r="B35" s="21"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
+      <c r="C35" s="22">
+        <v>43524</v>
+      </c>
+      <c r="D35" s="23">
+        <v>29.92</v>
+      </c>
+      <c r="E35" s="26">
+        <v>-1.93</v>
+      </c>
+      <c r="F35" s="26">
+        <v>8.32</v>
+      </c>
       <c r="G35" s="26"/>
-      <c r="H35" s="26"/>
+      <c r="H35" s="26">
+        <v>13.6</v>
+      </c>
     </row>
     <row r="36" ht="24.75" customHeight="1" spans="1:8">
       <c r="A36" s="25"/>
       <c r="B36" s="21"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
+      <c r="C36" s="22">
+        <v>43550</v>
+      </c>
+      <c r="D36" s="23">
+        <v>31.23</v>
+      </c>
+      <c r="E36" s="26">
+        <v>4.45</v>
+      </c>
+      <c r="F36" s="26">
+        <v>9.17</v>
+      </c>
       <c r="G36" s="26"/>
-      <c r="H36" s="26"/>
+      <c r="H36" s="26">
+        <v>13.42</v>
+      </c>
     </row>
     <row r="37" ht="24.75" customHeight="1" spans="1:8">
       <c r="A37" s="25"/>
@@ -3110,32 +3120,64 @@
     <row r="75" ht="24.75" customHeight="1" spans="1:8">
       <c r="A75" s="25"/>
       <c r="B75" s="36"/>
-      <c r="C75" s="49"/>
-      <c r="D75" s="47"/>
-      <c r="E75" s="26"/>
-      <c r="F75" s="26"/>
+      <c r="C75" s="22">
+        <v>43523</v>
+      </c>
+      <c r="D75" s="47">
+        <v>34.684</v>
+      </c>
+      <c r="E75" s="26">
+        <v>0.37</v>
+      </c>
+      <c r="F75" s="26">
+        <v>9.58</v>
+      </c>
       <c r="G75" s="26"/>
-      <c r="H75" s="44"/>
+      <c r="H75" s="44">
+        <v>19.69</v>
+      </c>
     </row>
     <row r="76" ht="24.75" customHeight="1" spans="1:8">
       <c r="A76" s="25"/>
       <c r="B76" s="36"/>
-      <c r="C76" s="49"/>
-      <c r="D76" s="47"/>
-      <c r="E76" s="26"/>
-      <c r="F76" s="26"/>
+      <c r="C76" s="22">
+        <v>43550</v>
+      </c>
+      <c r="D76" s="47">
+        <v>37.145</v>
+      </c>
+      <c r="E76" s="26">
+        <v>11.5</v>
+      </c>
+      <c r="F76" s="26">
+        <v>11.4</v>
+      </c>
       <c r="G76" s="26"/>
-      <c r="H76" s="44"/>
+      <c r="H76" s="44">
+        <v>19.7</v>
+      </c>
     </row>
     <row r="77" ht="24.75" customHeight="1" spans="1:8">
       <c r="A77" s="25"/>
       <c r="B77" s="36"/>
-      <c r="C77" s="49"/>
-      <c r="D77" s="47"/>
-      <c r="E77" s="26"/>
-      <c r="F77" s="26"/>
-      <c r="G77" s="26"/>
-      <c r="H77" s="44"/>
+      <c r="C77" s="22">
+        <v>43551</v>
+      </c>
+      <c r="D77" s="47">
+        <v>37.088</v>
+      </c>
+      <c r="E77" s="26">
+        <v>10.36</v>
+      </c>
+      <c r="F77" s="26">
+        <v>12.13</v>
+      </c>
+      <c r="G77" s="26">
+        <v>18.56</v>
+      </c>
+      <c r="H77" s="44">
+        <v>19.89</v>
+      </c>
     </row>
     <row r="78" ht="24.75" customHeight="1" spans="1:8">
       <c r="A78" s="25"/>
@@ -3152,533 +3194,533 @@
       <c r="B79" s="33"/>
     </row>
     <row r="80" ht="24.75" customHeight="1" spans="1:8">
-      <c r="A80" s="50" t="str">
+      <c r="A80" s="49" t="str">
         <f>HYPERLINK("http://www.moneycontrol.com/mutual-funds/nav/reliance-top-200-fund-direct-plan/MRC940","Reliance Top 200 Fund - Direct Plan (G). New name: Reliance Large Cap Fund - Direct Plan (G)")</f>
         <v>Reliance Top 200 Fund - Direct Plan (G). New name: Reliance Large Cap Fund - Direct Plan (G)</v>
       </c>
       <c r="B80" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C80" s="51">
+      <c r="C80" s="50">
         <v>43199</v>
       </c>
-      <c r="D80" s="52">
+      <c r="D80" s="51">
         <v>33.495</v>
       </c>
-      <c r="E80" s="53">
+      <c r="E80" s="52">
         <v>15.7</v>
       </c>
-      <c r="F80" s="53">
+      <c r="F80" s="52">
         <v>23</v>
       </c>
-      <c r="G80" s="53">
+      <c r="G80" s="52">
         <v>9.6</v>
       </c>
-      <c r="H80" s="53"/>
+      <c r="H80" s="52"/>
     </row>
     <row r="81" ht="24.75" customHeight="1" spans="1:8">
-      <c r="A81" s="50"/>
+      <c r="A81" s="49"/>
       <c r="B81" s="21"/>
-      <c r="C81" s="51">
+      <c r="C81" s="50">
         <v>43200</v>
       </c>
-      <c r="D81" s="52">
+      <c r="D81" s="51">
         <v>33.642</v>
       </c>
-      <c r="E81" s="53">
+      <c r="E81" s="52">
         <v>15.9</v>
       </c>
-      <c r="F81" s="53">
+      <c r="F81" s="52">
         <v>23.2</v>
       </c>
-      <c r="G81" s="53">
+      <c r="G81" s="52">
         <v>9.8</v>
       </c>
-      <c r="H81" s="53"/>
+      <c r="H81" s="52"/>
     </row>
     <row r="82" ht="24.75" customHeight="1" spans="1:8">
-      <c r="A82" s="50"/>
+      <c r="A82" s="49"/>
       <c r="B82" s="21"/>
-      <c r="C82" s="51">
+      <c r="C82" s="50">
         <v>43202</v>
       </c>
-      <c r="D82" s="52">
+      <c r="D82" s="51">
         <v>33.521</v>
       </c>
-      <c r="E82" s="54">
+      <c r="E82" s="53">
         <v>14.7</v>
       </c>
-      <c r="F82" s="54">
+      <c r="F82" s="53">
         <v>21.7</v>
       </c>
-      <c r="G82" s="54">
+      <c r="G82" s="53">
         <v>9.6</v>
       </c>
-      <c r="H82" s="54"/>
+      <c r="H82" s="53"/>
     </row>
     <row r="83" ht="24.75" customHeight="1" spans="1:8">
-      <c r="A83" s="50"/>
+      <c r="A83" s="49"/>
       <c r="B83" s="21"/>
-      <c r="C83" s="51">
+      <c r="C83" s="50">
         <v>43203</v>
       </c>
-      <c r="D83" s="52">
+      <c r="D83" s="51">
         <v>33.477</v>
       </c>
-      <c r="E83" s="54">
+      <c r="E83" s="53">
         <v>15.1</v>
       </c>
-      <c r="F83" s="54">
+      <c r="F83" s="53">
         <v>20.7</v>
       </c>
-      <c r="G83" s="54">
+      <c r="G83" s="53">
         <v>9.5</v>
       </c>
-      <c r="H83" s="54"/>
+      <c r="H83" s="53"/>
     </row>
     <row r="84" ht="24.75" customHeight="1" spans="1:8">
-      <c r="A84" s="50"/>
+      <c r="A84" s="49"/>
       <c r="B84" s="21"/>
-      <c r="C84" s="51">
+      <c r="C84" s="50">
         <v>43208</v>
       </c>
-      <c r="D84" s="52">
+      <c r="D84" s="51">
         <v>33.628</v>
       </c>
-      <c r="E84" s="54">
+      <c r="E84" s="53">
         <v>16.9</v>
       </c>
-      <c r="F84" s="54">
+      <c r="F84" s="53">
         <v>20.6</v>
       </c>
-      <c r="G84" s="54">
+      <c r="G84" s="53">
         <v>10.8</v>
       </c>
-      <c r="H84" s="54">
+      <c r="H84" s="53">
         <v>19.3</v>
       </c>
     </row>
     <row r="85" ht="24.75" customHeight="1" spans="1:8">
-      <c r="A85" s="50"/>
+      <c r="A85" s="49"/>
       <c r="B85" s="21"/>
-      <c r="C85" s="51">
+      <c r="C85" s="50">
         <v>43311</v>
       </c>
-      <c r="D85" s="55">
+      <c r="D85" s="54">
         <v>35.085</v>
       </c>
-      <c r="E85" s="56">
+      <c r="E85" s="55">
         <v>10.3</v>
       </c>
-      <c r="F85" s="56">
+      <c r="F85" s="55">
         <v>17.1</v>
       </c>
-      <c r="G85" s="56">
+      <c r="G85" s="55">
         <v>11.8</v>
       </c>
-      <c r="H85" s="56">
+      <c r="H85" s="55">
         <v>22.4</v>
       </c>
     </row>
     <row r="86" ht="24.75" customHeight="1" spans="1:8">
-      <c r="A86" s="50"/>
+      <c r="A86" s="49"/>
       <c r="B86" s="21"/>
-      <c r="C86" s="51">
+      <c r="C86" s="50">
         <v>43312</v>
       </c>
-      <c r="D86" s="52">
+      <c r="D86" s="51">
         <v>35.068</v>
       </c>
-      <c r="E86" s="56">
+      <c r="E86" s="55">
         <v>9.4</v>
       </c>
-      <c r="F86" s="56">
+      <c r="F86" s="55">
         <v>17.1</v>
       </c>
-      <c r="G86" s="56">
+      <c r="G86" s="55">
         <v>11.4</v>
       </c>
-      <c r="H86" s="56">
+      <c r="H86" s="55">
         <v>22.1</v>
       </c>
     </row>
     <row r="87" ht="24.75" customHeight="1" spans="1:8">
-      <c r="A87" s="50"/>
+      <c r="A87" s="49"/>
       <c r="B87" s="21"/>
-      <c r="C87" s="51">
+      <c r="C87" s="50">
         <v>43313</v>
       </c>
-      <c r="D87" s="55">
+      <c r="D87" s="54">
         <v>35.109</v>
       </c>
-      <c r="E87" s="56">
+      <c r="E87" s="55">
         <v>9.4</v>
       </c>
-      <c r="F87" s="56">
+      <c r="F87" s="55">
         <v>17.5</v>
       </c>
-      <c r="G87" s="56">
+      <c r="G87" s="55">
         <v>11.4</v>
       </c>
-      <c r="H87" s="56">
+      <c r="H87" s="55">
         <v>22.4</v>
       </c>
     </row>
     <row r="88" ht="24.75" customHeight="1" spans="1:8">
-      <c r="A88" s="50"/>
+      <c r="A88" s="49"/>
       <c r="B88" s="21"/>
-      <c r="C88" s="51">
+      <c r="C88" s="50">
         <v>43319</v>
       </c>
-      <c r="D88" s="52">
+      <c r="D88" s="51">
         <v>35.367</v>
       </c>
-      <c r="E88" s="56">
+      <c r="E88" s="55">
         <v>10.9</v>
       </c>
-      <c r="F88" s="56">
+      <c r="F88" s="55">
         <v>17.4</v>
       </c>
-      <c r="G88" s="56">
+      <c r="G88" s="55">
         <v>11.3</v>
       </c>
-      <c r="H88" s="56">
+      <c r="H88" s="55">
         <v>23.1</v>
       </c>
     </row>
     <row r="89" ht="24.75" customHeight="1" spans="1:8">
-      <c r="A89" s="50"/>
+      <c r="A89" s="49"/>
       <c r="B89" s="21"/>
-      <c r="C89" s="51">
+      <c r="C89" s="50">
         <v>43321</v>
       </c>
-      <c r="D89" s="52">
+      <c r="D89" s="51">
         <v>35.687</v>
       </c>
-      <c r="E89" s="56">
+      <c r="E89" s="55">
         <v>14.2</v>
       </c>
-      <c r="F89" s="56">
+      <c r="F89" s="55">
         <v>18</v>
       </c>
-      <c r="G89" s="56">
+      <c r="G89" s="55">
         <v>11.6</v>
       </c>
-      <c r="H89" s="56">
+      <c r="H89" s="55">
         <v>22.9</v>
       </c>
     </row>
     <row r="90" ht="24.75" customHeight="1" spans="1:8">
-      <c r="A90" s="50"/>
+      <c r="A90" s="49"/>
       <c r="B90" s="21"/>
-      <c r="C90" s="51">
+      <c r="C90" s="50">
         <v>43322</v>
       </c>
-      <c r="D90" s="52">
+      <c r="D90" s="51">
         <v>35.367</v>
       </c>
-      <c r="E90" s="56">
+      <c r="E90" s="55">
         <v>14.4</v>
       </c>
-      <c r="F90" s="56">
+      <c r="F90" s="55">
         <v>18.4</v>
       </c>
-      <c r="G90" s="56">
+      <c r="G90" s="55">
         <v>11.4</v>
       </c>
-      <c r="H90" s="56">
+      <c r="H90" s="55">
         <v>22.7</v>
       </c>
     </row>
     <row r="91" ht="24.75" customHeight="1" spans="1:8">
-      <c r="A91" s="50"/>
+      <c r="A91" s="49"/>
       <c r="B91" s="21"/>
-      <c r="C91" s="51">
+      <c r="C91" s="50">
         <v>43325</v>
       </c>
-      <c r="D91" s="52">
+      <c r="D91" s="51">
         <v>35.079</v>
       </c>
-      <c r="E91" s="56">
+      <c r="E91" s="55">
         <v>14.4</v>
       </c>
-      <c r="F91" s="56">
+      <c r="F91" s="55">
         <v>17.2</v>
       </c>
-      <c r="G91" s="56">
+      <c r="G91" s="55">
         <v>11.9</v>
       </c>
-      <c r="H91" s="56">
+      <c r="H91" s="55">
         <v>21.9</v>
       </c>
     </row>
     <row r="92" ht="24.75" customHeight="1" spans="1:8">
-      <c r="A92" s="50"/>
+      <c r="A92" s="49"/>
       <c r="B92" s="21"/>
-      <c r="C92" s="51">
+      <c r="C92" s="50">
         <v>43326</v>
       </c>
-      <c r="D92" s="52">
+      <c r="D92" s="51">
         <v>35.393</v>
       </c>
-      <c r="E92" s="56">
+      <c r="E92" s="55">
         <v>14.1</v>
       </c>
-      <c r="F92" s="56">
+      <c r="F92" s="55">
         <v>17.7</v>
       </c>
-      <c r="G92" s="56">
+      <c r="G92" s="55">
         <v>11.5</v>
       </c>
-      <c r="H92" s="56">
+      <c r="H92" s="55">
         <v>22</v>
       </c>
     </row>
     <row r="93" ht="24.75" customHeight="1" spans="1:8">
-      <c r="A93" s="50"/>
+      <c r="A93" s="49"/>
       <c r="B93" s="21"/>
-      <c r="C93" s="51">
+      <c r="C93" s="50">
         <v>43332</v>
       </c>
-      <c r="D93" s="52">
+      <c r="D93" s="51">
         <v>36.178</v>
       </c>
-      <c r="E93" s="56">
+      <c r="E93" s="55">
         <v>16.3</v>
       </c>
-      <c r="F93" s="56">
+      <c r="F93" s="55">
         <v>18</v>
       </c>
-      <c r="G93" s="56">
+      <c r="G93" s="55">
         <v>12.7</v>
       </c>
-      <c r="H93" s="56">
+      <c r="H93" s="55">
         <v>23.8</v>
       </c>
     </row>
     <row r="94" ht="24.75" customHeight="1" spans="1:8">
-      <c r="A94" s="50"/>
+      <c r="A94" s="49"/>
       <c r="B94" s="21"/>
-      <c r="C94" s="51">
+      <c r="C94" s="50">
         <v>43333</v>
       </c>
-      <c r="D94" s="52">
+      <c r="D94" s="51">
         <v>36.298</v>
       </c>
-      <c r="E94" s="56">
+      <c r="E94" s="55">
         <v>18</v>
       </c>
-      <c r="F94" s="56">
+      <c r="F94" s="55">
         <v>18.2</v>
       </c>
-      <c r="G94" s="56">
+      <c r="G94" s="55">
         <v>13.1</v>
       </c>
-      <c r="H94" s="56">
+      <c r="H94" s="55">
         <v>24.3</v>
       </c>
     </row>
     <row r="95" ht="24.75" customHeight="1" spans="1:8">
-      <c r="A95" s="50"/>
+      <c r="A95" s="49"/>
       <c r="B95" s="21"/>
-      <c r="C95" s="51">
+      <c r="C95" s="50">
         <v>43336</v>
       </c>
-      <c r="D95" s="52">
+      <c r="D95" s="51">
         <v>36.183</v>
       </c>
-      <c r="E95" s="56">
+      <c r="E95" s="55">
         <v>15.9</v>
       </c>
-      <c r="F95" s="56">
+      <c r="F95" s="55">
         <v>18</v>
       </c>
-      <c r="G95" s="56">
+      <c r="G95" s="55">
         <v>15.6</v>
       </c>
-      <c r="H95" s="56">
+      <c r="H95" s="55">
         <v>23.5</v>
       </c>
     </row>
     <row r="96" ht="24.75" customHeight="1" spans="1:8">
-      <c r="A96" s="50"/>
+      <c r="A96" s="49"/>
       <c r="B96" s="21"/>
-      <c r="C96" s="51">
+      <c r="C96" s="50">
         <v>43342</v>
       </c>
-      <c r="D96" s="52">
+      <c r="D96" s="51">
         <v>36.845</v>
       </c>
-      <c r="E96" s="56">
+      <c r="E96" s="55">
         <v>17.3</v>
       </c>
-      <c r="F96" s="56">
+      <c r="F96" s="55">
         <v>18.3</v>
       </c>
-      <c r="G96" s="56">
+      <c r="G96" s="55">
         <v>15.2</v>
       </c>
-      <c r="H96" s="56">
+      <c r="H96" s="55">
         <v>23.9</v>
       </c>
     </row>
     <row r="97" ht="24.75" customHeight="1" spans="1:8">
-      <c r="A97" s="50"/>
+      <c r="A97" s="49"/>
       <c r="B97" s="21"/>
-      <c r="C97" s="51">
+      <c r="C97" s="50">
         <v>43348</v>
       </c>
-      <c r="D97" s="52">
+      <c r="D97" s="51">
         <v>36.203</v>
       </c>
-      <c r="E97" s="56">
+      <c r="E97" s="55">
         <v>14.7</v>
       </c>
-      <c r="F97" s="56">
+      <c r="F97" s="55">
         <v>16.8</v>
       </c>
-      <c r="G97" s="56">
+      <c r="G97" s="55">
         <v>16.2</v>
       </c>
-      <c r="H97" s="56">
+      <c r="H97" s="55">
         <v>23.1</v>
       </c>
     </row>
     <row r="98" ht="24.75" customHeight="1" spans="1:8">
-      <c r="A98" s="50"/>
+      <c r="A98" s="49"/>
       <c r="B98" s="21"/>
-      <c r="C98" s="51">
+      <c r="C98" s="50">
         <v>43368</v>
       </c>
-      <c r="D98" s="52">
+      <c r="D98" s="51">
         <v>34.648</v>
       </c>
-      <c r="E98" s="56">
+      <c r="E98" s="55">
         <v>9.1</v>
       </c>
-      <c r="F98" s="56">
+      <c r="F98" s="55">
         <v>13.7</v>
       </c>
-      <c r="G98" s="56">
+      <c r="G98" s="55">
         <v>13.8</v>
       </c>
-      <c r="H98" s="56">
+      <c r="H98" s="55">
         <v>21</v>
       </c>
     </row>
     <row r="99" ht="24.75" customHeight="1" spans="1:8">
-      <c r="A99" s="50"/>
+      <c r="A99" s="49"/>
       <c r="B99" s="21"/>
-      <c r="C99" s="51">
+      <c r="C99" s="50">
         <v>43383</v>
       </c>
-      <c r="D99" s="52">
+      <c r="D99" s="51">
         <v>33.023</v>
       </c>
-      <c r="E99" s="56">
+      <c r="E99" s="55">
         <v>3.4</v>
       </c>
-      <c r="F99" s="56">
+      <c r="F99" s="55">
         <v>11.3</v>
       </c>
-      <c r="G99" s="56">
+      <c r="G99" s="55">
         <v>11.2</v>
       </c>
-      <c r="H99" s="56">
+      <c r="H99" s="55">
         <v>19.2</v>
       </c>
     </row>
     <row r="100" ht="24.75" customHeight="1" spans="1:8">
-      <c r="A100" s="50"/>
+      <c r="A100" s="49"/>
       <c r="B100" s="21"/>
-      <c r="C100" s="51">
+      <c r="C100" s="50">
         <v>43399</v>
       </c>
-      <c r="D100" s="57">
+      <c r="D100" s="56">
         <v>31.994</v>
       </c>
-      <c r="E100" s="58">
+      <c r="E100" s="57">
         <v>-3.3</v>
       </c>
-      <c r="F100" s="58">
+      <c r="F100" s="57">
         <v>9.8</v>
       </c>
-      <c r="G100" s="58">
+      <c r="G100" s="57">
         <v>9.5</v>
       </c>
-      <c r="H100" s="58">
+      <c r="H100" s="57">
         <v>18</v>
       </c>
     </row>
     <row r="101" ht="24.75" customHeight="1" spans="1:8">
-      <c r="A101" s="50"/>
+      <c r="A101" s="49"/>
       <c r="B101" s="21"/>
-      <c r="C101" s="51">
+      <c r="C101" s="50">
         <v>43402</v>
       </c>
-      <c r="D101" s="55">
+      <c r="D101" s="54">
         <v>33.094</v>
       </c>
-      <c r="E101" s="56">
+      <c r="E101" s="55">
         <v>0.1</v>
       </c>
-      <c r="F101" s="56">
+      <c r="F101" s="55">
         <v>11.7</v>
       </c>
-      <c r="G101" s="56">
+      <c r="G101" s="55">
         <v>11.4</v>
       </c>
-      <c r="H101" s="56">
+      <c r="H101" s="55">
         <v>18.6</v>
       </c>
     </row>
     <row r="102" ht="24.75" customHeight="1" spans="1:8">
-      <c r="A102" s="50"/>
+      <c r="A102" s="49"/>
       <c r="B102" s="21"/>
-      <c r="C102" s="51"/>
-      <c r="D102" s="52"/>
-      <c r="E102" s="56"/>
-      <c r="F102" s="56"/>
-      <c r="G102" s="56"/>
-      <c r="H102" s="56"/>
+      <c r="C102" s="50"/>
+      <c r="D102" s="51"/>
+      <c r="E102" s="55"/>
+      <c r="F102" s="55"/>
+      <c r="G102" s="55"/>
+      <c r="H102" s="55"/>
     </row>
     <row r="103" ht="24.75" customHeight="1" spans="1:8">
-      <c r="A103" s="50"/>
+      <c r="A103" s="49"/>
       <c r="B103" s="21"/>
-      <c r="C103" s="51"/>
-      <c r="D103" s="52"/>
-      <c r="E103" s="56"/>
-      <c r="F103" s="56"/>
-      <c r="G103" s="56"/>
-      <c r="H103" s="56"/>
+      <c r="C103" s="50"/>
+      <c r="D103" s="51"/>
+      <c r="E103" s="55"/>
+      <c r="F103" s="55"/>
+      <c r="G103" s="55"/>
+      <c r="H103" s="55"/>
     </row>
     <row r="104" ht="24.75" customHeight="1" spans="1:8">
-      <c r="A104" s="50"/>
+      <c r="A104" s="49"/>
       <c r="B104" s="21"/>
-      <c r="C104" s="51"/>
-      <c r="D104" s="52"/>
-      <c r="E104" s="56"/>
-      <c r="F104" s="56"/>
-      <c r="G104" s="56"/>
-      <c r="H104" s="56"/>
+      <c r="C104" s="50"/>
+      <c r="D104" s="51"/>
+      <c r="E104" s="55"/>
+      <c r="F104" s="55"/>
+      <c r="G104" s="55"/>
+      <c r="H104" s="55"/>
     </row>
     <row r="105" ht="24.75" customHeight="1" spans="1:8">
-      <c r="A105" s="50"/>
+      <c r="A105" s="49"/>
       <c r="B105" s="21"/>
-      <c r="C105" s="51"/>
-      <c r="D105" s="52"/>
-      <c r="E105" s="56"/>
-      <c r="F105" s="56"/>
-      <c r="G105" s="56"/>
-      <c r="H105" s="56"/>
+      <c r="C105" s="50"/>
+      <c r="D105" s="51"/>
+      <c r="E105" s="55"/>
+      <c r="F105" s="55"/>
+      <c r="G105" s="55"/>
+      <c r="H105" s="55"/>
     </row>
     <row r="106" ht="24.75" customHeight="1" spans="3:8">
-      <c r="C106" s="59"/>
-      <c r="D106" s="60"/>
-      <c r="E106" s="61"/>
-      <c r="F106" s="61"/>
-      <c r="G106" s="61"/>
-      <c r="H106" s="61"/>
+      <c r="C106" s="58"/>
+      <c r="D106" s="59"/>
+      <c r="E106" s="60"/>
+      <c r="F106" s="60"/>
+      <c r="G106" s="60"/>
+      <c r="H106" s="60"/>
     </row>
     <row r="107" ht="24.75" customHeight="1" spans="1:8">
       <c r="A107" s="25" t="str">
@@ -3694,16 +3736,16 @@
       <c r="D107" s="23">
         <v>23.422</v>
       </c>
-      <c r="E107" s="62">
+      <c r="E107" s="61">
         <v>10.2</v>
       </c>
-      <c r="F107" s="62">
+      <c r="F107" s="61">
         <v>17.6</v>
       </c>
-      <c r="G107" s="62">
+      <c r="G107" s="61">
         <v>8.4</v>
       </c>
-      <c r="H107" s="62"/>
+      <c r="H107" s="61"/>
     </row>
     <row r="108" ht="24.75" customHeight="1" spans="1:8">
       <c r="A108" s="25"/>
@@ -3714,16 +3756,16 @@
       <c r="D108" s="23">
         <v>23.421</v>
       </c>
-      <c r="E108" s="62">
+      <c r="E108" s="61">
         <v>10.8</v>
       </c>
-      <c r="F108" s="62">
+      <c r="F108" s="61">
         <v>16.8</v>
       </c>
-      <c r="G108" s="62">
+      <c r="G108" s="61">
         <v>8.5</v>
       </c>
-      <c r="H108" s="63"/>
+      <c r="H108" s="62"/>
     </row>
     <row r="109" ht="24.75" customHeight="1" spans="1:8">
       <c r="A109" s="25"/>
@@ -3734,16 +3776,16 @@
       <c r="D109" s="23">
         <v>23.551</v>
       </c>
-      <c r="E109" s="62">
+      <c r="E109" s="61">
         <v>11.8</v>
       </c>
-      <c r="F109" s="62">
+      <c r="F109" s="61">
         <v>17.1</v>
       </c>
-      <c r="G109" s="62">
+      <c r="G109" s="61">
         <v>9.7</v>
       </c>
-      <c r="H109" s="62">
+      <c r="H109" s="61">
         <v>18.4</v>
       </c>
     </row>
@@ -3756,16 +3798,16 @@
       <c r="D110" s="23">
         <v>23.494</v>
       </c>
-      <c r="E110" s="62">
+      <c r="E110" s="61">
         <v>11.9</v>
       </c>
-      <c r="F110" s="62">
+      <c r="F110" s="61">
         <v>16.4</v>
       </c>
-      <c r="G110" s="62">
+      <c r="G110" s="61">
         <v>9.6</v>
       </c>
-      <c r="H110" s="62">
+      <c r="H110" s="61">
         <v>18.2</v>
       </c>
     </row>
@@ -3781,7 +3823,7 @@
       <c r="E111" s="26">
         <v>5.8</v>
       </c>
-      <c r="F111" s="62"/>
+      <c r="F111" s="61"/>
       <c r="G111" s="26">
         <v>10.5</v>
       </c>
@@ -4322,22 +4364,42 @@
     <row r="137" ht="24.75" customHeight="1" spans="1:8">
       <c r="A137" s="25"/>
       <c r="B137" s="21"/>
-      <c r="C137" s="22"/>
-      <c r="D137" s="23"/>
-      <c r="E137" s="26"/>
-      <c r="F137" s="26"/>
+      <c r="C137" s="22">
+        <v>43524</v>
+      </c>
+      <c r="D137" s="23">
+        <v>22.032</v>
+      </c>
+      <c r="E137" s="26">
+        <v>-5.41</v>
+      </c>
+      <c r="F137" s="26">
+        <v>4.84</v>
+      </c>
       <c r="G137" s="26"/>
-      <c r="H137" s="26"/>
+      <c r="H137" s="26">
+        <v>15.3</v>
+      </c>
     </row>
     <row r="138" ht="24.75" customHeight="1" spans="1:8">
       <c r="A138" s="25"/>
       <c r="B138" s="21"/>
-      <c r="C138" s="22"/>
-      <c r="D138" s="23"/>
-      <c r="E138" s="26"/>
-      <c r="F138" s="26"/>
+      <c r="C138" s="22">
+        <v>43550</v>
+      </c>
+      <c r="D138" s="23">
+        <v>23.762</v>
+      </c>
+      <c r="E138" s="26">
+        <v>6.1</v>
+      </c>
+      <c r="F138" s="26">
+        <v>6.42</v>
+      </c>
       <c r="G138" s="26"/>
-      <c r="H138" s="26"/>
+      <c r="H138" s="26">
+        <v>15.67</v>
+      </c>
     </row>
     <row r="139" ht="24.75" customHeight="1" spans="1:8">
       <c r="A139" s="25"/>
@@ -4354,10 +4416,10 @@
       <c r="B140" s="21"/>
       <c r="C140" s="22"/>
       <c r="D140" s="23"/>
-      <c r="E140" s="62"/>
-      <c r="F140" s="62"/>
-      <c r="G140" s="62"/>
-      <c r="H140" s="62"/>
+      <c r="E140" s="61"/>
+      <c r="F140" s="61"/>
+      <c r="G140" s="61"/>
+      <c r="H140" s="61"/>
     </row>
     <row r="141" ht="24.75" customHeight="1"/>
     <row r="142" ht="24.75" customHeight="1" spans="1:8">
@@ -4374,16 +4436,16 @@
       <c r="D142" s="23">
         <v>42.529</v>
       </c>
-      <c r="E142" s="62">
+      <c r="E142" s="61">
         <v>29.3</v>
       </c>
-      <c r="F142" s="62">
+      <c r="F142" s="61">
         <v>28.9</v>
       </c>
-      <c r="G142" s="62">
+      <c r="G142" s="61">
         <v>13.1</v>
       </c>
-      <c r="H142" s="62"/>
+      <c r="H142" s="61"/>
     </row>
     <row r="143" ht="24.75" customHeight="1" spans="1:8">
       <c r="A143" s="25"/>
@@ -4394,16 +4456,16 @@
       <c r="D143" s="23">
         <v>42.575</v>
       </c>
-      <c r="E143" s="62">
+      <c r="E143" s="61">
         <v>30.1</v>
       </c>
-      <c r="F143" s="62">
+      <c r="F143" s="61">
         <v>28.5</v>
       </c>
-      <c r="G143" s="62">
+      <c r="G143" s="61">
         <v>14.2</v>
       </c>
-      <c r="H143" s="62">
+      <c r="H143" s="61">
         <v>17.6</v>
       </c>
     </row>
@@ -4960,22 +5022,42 @@
     <row r="169" ht="24.75" customHeight="1" spans="1:8">
       <c r="A169" s="25"/>
       <c r="B169" s="21"/>
-      <c r="C169" s="22"/>
-      <c r="D169" s="31"/>
-      <c r="E169" s="26"/>
-      <c r="F169" s="26"/>
+      <c r="C169" s="22">
+        <v>43524</v>
+      </c>
+      <c r="D169" s="31">
+        <v>37.05</v>
+      </c>
+      <c r="E169" s="26">
+        <v>-11.48</v>
+      </c>
+      <c r="F169" s="26">
+        <v>10.52</v>
+      </c>
       <c r="G169" s="26"/>
-      <c r="H169" s="26"/>
+      <c r="H169" s="26">
+        <v>12.29</v>
+      </c>
     </row>
     <row r="170" ht="24.75" customHeight="1" spans="1:8">
       <c r="A170" s="25"/>
       <c r="B170" s="21"/>
-      <c r="C170" s="22"/>
-      <c r="D170" s="31"/>
-      <c r="E170" s="26"/>
-      <c r="F170" s="26"/>
+      <c r="C170" s="22">
+        <v>43550</v>
+      </c>
+      <c r="D170" s="31">
+        <v>38.64</v>
+      </c>
+      <c r="E170" s="26">
+        <v>-4.62</v>
+      </c>
+      <c r="F170" s="26">
+        <v>11.53</v>
+      </c>
       <c r="G170" s="26"/>
-      <c r="H170" s="26"/>
+      <c r="H170" s="26">
+        <v>12.56</v>
+      </c>
     </row>
     <row r="171" ht="24.75" customHeight="1" spans="1:8">
       <c r="A171" s="25"/>
@@ -5092,16 +5174,16 @@
       <c r="D179" s="23">
         <v>48.617</v>
       </c>
-      <c r="E179" s="62">
+      <c r="E179" s="61">
         <v>35.3</v>
       </c>
-      <c r="F179" s="62">
+      <c r="F179" s="61">
         <v>35.1</v>
       </c>
-      <c r="G179" s="62">
+      <c r="G179" s="61">
         <v>21.2</v>
       </c>
-      <c r="H179" s="62"/>
+      <c r="H179" s="61"/>
     </row>
     <row r="180" ht="24.75" customHeight="1" spans="1:8">
       <c r="A180" s="25"/>
@@ -5112,16 +5194,16 @@
       <c r="D180" s="23">
         <v>48.889</v>
       </c>
-      <c r="E180" s="62">
+      <c r="E180" s="61">
         <v>36.1</v>
       </c>
-      <c r="F180" s="62">
+      <c r="F180" s="61">
         <v>34.6</v>
       </c>
-      <c r="G180" s="62">
+      <c r="G180" s="61">
         <v>21.1</v>
       </c>
-      <c r="H180" s="62"/>
+      <c r="H180" s="61"/>
     </row>
     <row r="181" ht="25" customHeight="1" spans="1:8">
       <c r="A181" s="25"/>
@@ -5132,16 +5214,16 @@
       <c r="D181" s="23">
         <v>49.202</v>
       </c>
-      <c r="E181" s="62">
+      <c r="E181" s="61">
         <v>37.5</v>
       </c>
-      <c r="F181" s="62">
+      <c r="F181" s="61">
         <v>34.4</v>
       </c>
-      <c r="G181" s="62">
+      <c r="G181" s="61">
         <v>22</v>
       </c>
-      <c r="H181" s="64">
+      <c r="H181" s="63">
         <v>26.8</v>
       </c>
     </row>
@@ -5217,7 +5299,7 @@
       <c r="C185" s="22">
         <v>43319</v>
       </c>
-      <c r="D185" s="65">
+      <c r="D185" s="64">
         <v>47.498</v>
       </c>
       <c r="E185" s="26">
@@ -5239,7 +5321,7 @@
       <c r="C186" s="22">
         <v>43321</v>
       </c>
-      <c r="D186" s="65">
+      <c r="D186" s="64">
         <v>47.795</v>
       </c>
       <c r="E186" s="26">
@@ -5261,7 +5343,7 @@
       <c r="C187" s="22">
         <v>43322</v>
       </c>
-      <c r="D187" s="65"/>
+      <c r="D187" s="64"/>
       <c r="E187" s="26">
         <v>26</v>
       </c>
@@ -5281,7 +5363,7 @@
       <c r="C188" s="22">
         <v>43325</v>
       </c>
-      <c r="D188" s="65">
+      <c r="D188" s="64">
         <v>47.119</v>
       </c>
       <c r="E188" s="26">
@@ -5325,16 +5407,16 @@
       <c r="C190" s="22">
         <v>43332</v>
       </c>
-      <c r="D190" s="65">
+      <c r="D190" s="64">
         <v>47.649</v>
       </c>
-      <c r="E190" s="66">
+      <c r="E190" s="65">
         <v>23.1</v>
       </c>
-      <c r="F190" s="66">
+      <c r="F190" s="65">
         <v>24</v>
       </c>
-      <c r="G190" s="66">
+      <c r="G190" s="65">
         <v>19.9</v>
       </c>
       <c r="H190" s="44">
@@ -5347,7 +5429,7 @@
       <c r="C191" s="22">
         <v>43333</v>
       </c>
-      <c r="D191" s="65">
+      <c r="D191" s="64">
         <v>47.867</v>
       </c>
       <c r="E191" s="26">
@@ -5369,7 +5451,7 @@
       <c r="C192" s="22">
         <v>43336</v>
       </c>
-      <c r="D192" s="65">
+      <c r="D192" s="64">
         <v>47.891</v>
       </c>
       <c r="E192" s="26">
@@ -5391,7 +5473,7 @@
       <c r="C193" s="22">
         <v>43342</v>
       </c>
-      <c r="D193" s="65">
+      <c r="D193" s="64">
         <v>48.772</v>
       </c>
       <c r="E193" s="26">
@@ -5413,7 +5495,7 @@
       <c r="C194" s="22">
         <v>43348</v>
       </c>
-      <c r="D194" s="65">
+      <c r="D194" s="64">
         <v>48.072</v>
       </c>
       <c r="E194" s="26">
@@ -5435,7 +5517,7 @@
       <c r="C195" s="22">
         <v>43368</v>
       </c>
-      <c r="D195" s="65">
+      <c r="D195" s="64">
         <v>45.432</v>
       </c>
       <c r="E195" s="26">
@@ -5457,7 +5539,7 @@
       <c r="C196" s="22">
         <v>43383</v>
       </c>
-      <c r="D196" s="65">
+      <c r="D196" s="64">
         <v>43.479</v>
       </c>
       <c r="E196" s="26">
@@ -5611,7 +5693,7 @@
       <c r="C203" s="22">
         <v>43430</v>
       </c>
-      <c r="D203" s="65">
+      <c r="D203" s="64">
         <v>44.374</v>
       </c>
       <c r="E203" s="26">
@@ -5655,7 +5737,7 @@
       <c r="C205" s="22">
         <v>43452</v>
       </c>
-      <c r="D205" s="65">
+      <c r="D205" s="64">
         <v>45.086</v>
       </c>
       <c r="E205" s="26">
@@ -5677,7 +5759,7 @@
       <c r="C206" s="22">
         <v>43461</v>
       </c>
-      <c r="D206" s="65">
+      <c r="D206" s="64">
         <v>44.788</v>
       </c>
       <c r="E206" s="26">
@@ -5699,7 +5781,7 @@
       <c r="C207" s="22">
         <v>43480</v>
       </c>
-      <c r="D207" s="65">
+      <c r="D207" s="64">
         <v>45.533</v>
       </c>
       <c r="E207" s="26">
@@ -5721,57 +5803,89 @@
       <c r="C208" s="22">
         <v>43511</v>
       </c>
-      <c r="D208" s="65">
+      <c r="D208" s="64">
         <v>42.503</v>
       </c>
-      <c r="E208" s="67">
+      <c r="E208" s="66">
         <v>-12.5</v>
       </c>
-      <c r="F208" s="67">
+      <c r="F208" s="66">
         <v>14.9</v>
       </c>
-      <c r="G208" s="67">
+      <c r="G208" s="66">
         <v>20.6</v>
       </c>
-      <c r="H208" s="68">
+      <c r="H208" s="67">
         <v>21</v>
       </c>
     </row>
     <row r="209" ht="25" customHeight="1" spans="1:8">
       <c r="A209" s="25"/>
       <c r="B209" s="36"/>
-      <c r="C209" s="22"/>
-      <c r="D209" s="65"/>
-      <c r="E209" s="26"/>
-      <c r="F209" s="26"/>
+      <c r="C209" s="22">
+        <v>43524</v>
+      </c>
+      <c r="D209" s="64">
+        <v>43.329</v>
+      </c>
+      <c r="E209" s="26">
+        <v>-9.96</v>
+      </c>
+      <c r="F209" s="26">
+        <v>14.81</v>
+      </c>
       <c r="G209" s="26"/>
-      <c r="H209" s="44"/>
+      <c r="H209" s="44">
+        <v>20.78</v>
+      </c>
     </row>
     <row r="210" ht="25" customHeight="1" spans="1:8">
       <c r="A210" s="25"/>
       <c r="B210" s="36"/>
-      <c r="C210" s="22"/>
-      <c r="D210" s="65"/>
-      <c r="E210" s="26"/>
-      <c r="F210" s="26"/>
+      <c r="C210" s="22">
+        <v>43550</v>
+      </c>
+      <c r="D210" s="64">
+        <v>46.607</v>
+      </c>
+      <c r="E210" s="26">
+        <v>0.4</v>
+      </c>
+      <c r="F210" s="26">
+        <v>16.16</v>
+      </c>
       <c r="G210" s="26"/>
-      <c r="H210" s="44"/>
+      <c r="H210" s="44">
+        <v>20.89</v>
+      </c>
     </row>
     <row r="211" ht="25" customHeight="1" spans="1:8">
       <c r="A211" s="25"/>
       <c r="B211" s="36"/>
-      <c r="C211" s="22"/>
-      <c r="D211" s="65"/>
-      <c r="E211" s="26"/>
-      <c r="F211" s="26"/>
-      <c r="G211" s="26"/>
-      <c r="H211" s="44"/>
+      <c r="C211" s="22">
+        <v>43551</v>
+      </c>
+      <c r="D211" s="64">
+        <v>47.462</v>
+      </c>
+      <c r="E211" s="26">
+        <v>1.8</v>
+      </c>
+      <c r="F211" s="26">
+        <v>17.85</v>
+      </c>
+      <c r="G211" s="26">
+        <v>23.17</v>
+      </c>
+      <c r="H211" s="44">
+        <v>21.15</v>
+      </c>
     </row>
     <row r="212" ht="25" customHeight="1" spans="1:8">
       <c r="A212" s="25"/>
       <c r="B212" s="36"/>
       <c r="C212" s="22"/>
-      <c r="D212" s="65"/>
+      <c r="D212" s="64"/>
       <c r="E212" s="26"/>
       <c r="F212" s="26"/>
       <c r="G212" s="26"/>
@@ -5780,16 +5894,16 @@
     <row r="213" ht="25" customHeight="1" spans="1:8">
       <c r="A213" s="25"/>
       <c r="B213" s="36"/>
-      <c r="C213" s="69"/>
-      <c r="D213" s="69"/>
-      <c r="E213" s="70"/>
-      <c r="F213" s="70"/>
-      <c r="G213" s="70"/>
-      <c r="H213" s="71"/>
+      <c r="C213" s="68"/>
+      <c r="D213" s="68"/>
+      <c r="E213" s="69"/>
+      <c r="F213" s="69"/>
+      <c r="G213" s="69"/>
+      <c r="H213" s="70"/>
     </row>
     <row r="214" ht="25" customHeight="1"/>
-    <row r="215" ht="25" customHeight="1" spans="1:8">
-      <c r="A215" s="72" t="s">
+    <row r="215" ht="25" customHeight="1" spans="1:9">
+      <c r="A215" s="71" t="s">
         <v>12</v>
       </c>
       <c r="B215" s="21" t="s">
@@ -5798,29 +5912,32 @@
       <c r="C215" s="22">
         <v>43313</v>
       </c>
-      <c r="D215" s="73">
+      <c r="D215" s="72">
         <v>35.109</v>
       </c>
-      <c r="E215" s="74">
+      <c r="E215" s="73">
         <v>9.4</v>
       </c>
-      <c r="F215" s="74">
+      <c r="F215" s="73">
         <v>17.5</v>
       </c>
-      <c r="G215" s="74">
+      <c r="G215" s="73">
         <v>11.4</v>
       </c>
-      <c r="H215" s="75">
+      <c r="H215" s="74">
         <v>22.4</v>
       </c>
+      <c r="I215" s="78" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="216" ht="25" customHeight="1" spans="1:8">
-      <c r="A216" s="72"/>
+      <c r="A216" s="71"/>
       <c r="B216" s="21"/>
       <c r="C216" s="22">
         <v>43319</v>
       </c>
-      <c r="D216" s="65">
+      <c r="D216" s="64">
         <v>35.367</v>
       </c>
       <c r="E216" s="26">
@@ -5837,12 +5954,12 @@
       </c>
     </row>
     <row r="217" ht="25" customHeight="1" spans="1:8">
-      <c r="A217" s="72"/>
+      <c r="A217" s="71"/>
       <c r="B217" s="21"/>
       <c r="C217" s="22">
         <v>43321</v>
       </c>
-      <c r="D217" s="65">
+      <c r="D217" s="64">
         <v>35.687</v>
       </c>
       <c r="E217" s="26">
@@ -5859,12 +5976,12 @@
       </c>
     </row>
     <row r="218" ht="25" customHeight="1" spans="1:8">
-      <c r="A218" s="72"/>
+      <c r="A218" s="71"/>
       <c r="B218" s="21"/>
       <c r="C218" s="22">
         <v>43322</v>
       </c>
-      <c r="D218" s="65">
+      <c r="D218" s="64">
         <v>35.367</v>
       </c>
       <c r="E218" s="26">
@@ -5881,12 +5998,12 @@
       </c>
     </row>
     <row r="219" ht="25" customHeight="1" spans="1:8">
-      <c r="A219" s="72"/>
+      <c r="A219" s="71"/>
       <c r="B219" s="21"/>
       <c r="C219" s="22">
         <v>43325</v>
       </c>
-      <c r="D219" s="65">
+      <c r="D219" s="64">
         <v>35.079</v>
       </c>
       <c r="E219" s="26">
@@ -5903,12 +6020,12 @@
       </c>
     </row>
     <row r="220" ht="25" customHeight="1" spans="1:8">
-      <c r="A220" s="72"/>
+      <c r="A220" s="71"/>
       <c r="B220" s="21"/>
       <c r="C220" s="22">
         <v>43326</v>
       </c>
-      <c r="D220" s="65">
+      <c r="D220" s="64">
         <v>35.393</v>
       </c>
       <c r="E220" s="26">
@@ -5925,12 +6042,12 @@
       </c>
     </row>
     <row r="221" ht="25" customHeight="1" spans="1:8">
-      <c r="A221" s="72"/>
+      <c r="A221" s="71"/>
       <c r="B221" s="21"/>
       <c r="C221" s="22">
         <v>43332</v>
       </c>
-      <c r="D221" s="65">
+      <c r="D221" s="64">
         <v>36.178</v>
       </c>
       <c r="E221" s="26">
@@ -5947,12 +6064,12 @@
       </c>
     </row>
     <row r="222" ht="25" customHeight="1" spans="1:8">
-      <c r="A222" s="72"/>
+      <c r="A222" s="71"/>
       <c r="B222" s="21"/>
       <c r="C222" s="22">
         <v>43333</v>
       </c>
-      <c r="D222" s="65">
+      <c r="D222" s="64">
         <v>36.298</v>
       </c>
       <c r="E222" s="26">
@@ -5969,12 +6086,12 @@
       </c>
     </row>
     <row r="223" ht="25" customHeight="1" spans="1:8">
-      <c r="A223" s="72"/>
+      <c r="A223" s="71"/>
       <c r="B223" s="21"/>
       <c r="C223" s="22">
         <v>43336</v>
       </c>
-      <c r="D223" s="65">
+      <c r="D223" s="64">
         <v>36.183</v>
       </c>
       <c r="E223" s="26">
@@ -5991,12 +6108,12 @@
       </c>
     </row>
     <row r="224" ht="25" customHeight="1" spans="1:8">
-      <c r="A224" s="72"/>
+      <c r="A224" s="71"/>
       <c r="B224" s="21"/>
       <c r="C224" s="22">
         <v>43342</v>
       </c>
-      <c r="D224" s="65">
+      <c r="D224" s="64">
         <v>36.845</v>
       </c>
       <c r="E224" s="26">
@@ -6013,12 +6130,12 @@
       </c>
     </row>
     <row r="225" ht="25" customHeight="1" spans="1:8">
-      <c r="A225" s="72"/>
+      <c r="A225" s="71"/>
       <c r="B225" s="21"/>
       <c r="C225" s="22">
         <v>43348</v>
       </c>
-      <c r="D225" s="65">
+      <c r="D225" s="64">
         <v>36.203</v>
       </c>
       <c r="E225" s="26">
@@ -6035,12 +6152,12 @@
       </c>
     </row>
     <row r="226" ht="25" customHeight="1" spans="1:8">
-      <c r="A226" s="72"/>
+      <c r="A226" s="71"/>
       <c r="B226" s="21"/>
       <c r="C226" s="22">
         <v>43368</v>
       </c>
-      <c r="D226" s="65">
+      <c r="D226" s="64">
         <v>34.648</v>
       </c>
       <c r="E226" s="26">
@@ -6057,12 +6174,12 @@
       </c>
     </row>
     <row r="227" ht="25" customHeight="1" spans="1:8">
-      <c r="A227" s="72"/>
+      <c r="A227" s="71"/>
       <c r="B227" s="21"/>
       <c r="C227" s="22">
         <v>43383</v>
       </c>
-      <c r="D227" s="65">
+      <c r="D227" s="64">
         <v>33.023</v>
       </c>
       <c r="E227" s="32">
@@ -6074,12 +6191,12 @@
       <c r="G227" s="32">
         <v>11.2</v>
       </c>
-      <c r="H227" s="76">
+      <c r="H227" s="75">
         <v>19.2</v>
       </c>
     </row>
     <row r="228" ht="25" customHeight="1" spans="1:8">
-      <c r="A228" s="72"/>
+      <c r="A228" s="71"/>
       <c r="B228" s="21"/>
       <c r="C228" s="22">
         <v>43399</v>
@@ -6101,7 +6218,7 @@
       </c>
     </row>
     <row r="229" ht="25" customHeight="1" spans="1:8">
-      <c r="A229" s="72"/>
+      <c r="A229" s="71"/>
       <c r="B229" s="21"/>
       <c r="C229" s="22">
         <v>43402</v>
@@ -6123,7 +6240,7 @@
       </c>
     </row>
     <row r="230" ht="25" customHeight="1" spans="1:8">
-      <c r="A230" s="72"/>
+      <c r="A230" s="71"/>
       <c r="B230" s="21"/>
       <c r="C230" s="22">
         <v>43404</v>
@@ -6145,7 +6262,7 @@
       </c>
     </row>
     <row r="231" ht="25" customHeight="1" spans="1:8">
-      <c r="A231" s="72"/>
+      <c r="A231" s="71"/>
       <c r="B231" s="21"/>
       <c r="C231" s="22">
         <v>43405</v>
@@ -6167,7 +6284,7 @@
       </c>
     </row>
     <row r="232" ht="25" customHeight="1" spans="1:8">
-      <c r="A232" s="72"/>
+      <c r="A232" s="71"/>
       <c r="B232" s="21"/>
       <c r="C232" s="22">
         <v>43410</v>
@@ -6189,7 +6306,7 @@
       </c>
     </row>
     <row r="233" ht="25" customHeight="1" spans="1:8">
-      <c r="A233" s="72"/>
+      <c r="A233" s="71"/>
       <c r="B233" s="21"/>
       <c r="C233" s="22">
         <v>43413</v>
@@ -6211,7 +6328,7 @@
       </c>
     </row>
     <row r="234" ht="25" customHeight="1" spans="1:8">
-      <c r="A234" s="72"/>
+      <c r="A234" s="71"/>
       <c r="B234" s="21"/>
       <c r="C234" s="22">
         <v>43430</v>
@@ -6233,7 +6350,7 @@
       </c>
     </row>
     <row r="235" ht="25" customHeight="1" spans="1:8">
-      <c r="A235" s="72"/>
+      <c r="A235" s="71"/>
       <c r="B235" s="21"/>
       <c r="C235" s="22">
         <v>43432</v>
@@ -6255,12 +6372,12 @@
       </c>
     </row>
     <row r="236" ht="25" customHeight="1" spans="1:8">
-      <c r="A236" s="72"/>
+      <c r="A236" s="71"/>
       <c r="B236" s="21"/>
       <c r="C236" s="22">
         <v>43452</v>
       </c>
-      <c r="D236" s="65">
+      <c r="D236" s="64">
         <v>34.937</v>
       </c>
       <c r="E236" s="26">
@@ -6277,12 +6394,12 @@
       </c>
     </row>
     <row r="237" ht="25" customHeight="1" spans="1:8">
-      <c r="A237" s="72"/>
+      <c r="A237" s="71"/>
       <c r="B237" s="21"/>
       <c r="C237" s="22">
         <v>43461</v>
       </c>
-      <c r="D237" s="65">
+      <c r="D237" s="64">
         <v>34.676</v>
       </c>
       <c r="E237" s="26">
@@ -6299,12 +6416,12 @@
       </c>
     </row>
     <row r="238" ht="25" customHeight="1" spans="1:8">
-      <c r="A238" s="72"/>
+      <c r="A238" s="71"/>
       <c r="B238" s="21"/>
       <c r="C238" s="22">
         <v>43480</v>
       </c>
-      <c r="D238" s="65">
+      <c r="D238" s="64">
         <v>35.366</v>
       </c>
       <c r="E238" s="26">
@@ -6321,779 +6438,912 @@
       </c>
     </row>
     <row r="239" ht="25" customHeight="1" spans="1:8">
-      <c r="A239" s="72"/>
+      <c r="A239" s="71"/>
       <c r="B239" s="21"/>
-      <c r="C239" s="22"/>
-      <c r="D239" s="65"/>
-      <c r="E239" s="32"/>
-      <c r="F239" s="32"/>
-      <c r="G239" s="32"/>
-      <c r="H239" s="76"/>
+      <c r="C239" s="22">
+        <v>43524</v>
+      </c>
+      <c r="D239" s="64">
+        <v>34.3414</v>
+      </c>
+      <c r="E239" s="32">
+        <v>0.87</v>
+      </c>
+      <c r="F239" s="32">
+        <v>11.56</v>
+      </c>
+      <c r="G239" s="32">
+        <v>19.11</v>
+      </c>
+      <c r="H239" s="75">
+        <v>17.64</v>
+      </c>
     </row>
     <row r="240" ht="25" customHeight="1" spans="1:8">
-      <c r="A240" s="72"/>
+      <c r="A240" s="71"/>
       <c r="B240" s="21"/>
-      <c r="C240" s="69"/>
-      <c r="D240" s="69"/>
-      <c r="E240" s="70"/>
-      <c r="F240" s="70"/>
-      <c r="G240" s="70"/>
-      <c r="H240" s="71"/>
-    </row>
-    <row r="241" ht="25" customHeight="1"/>
+      <c r="C240" s="22">
+        <v>43550</v>
+      </c>
+      <c r="D240" s="64">
+        <v>36.7706</v>
+      </c>
+      <c r="E240" s="32">
+        <v>13.88</v>
+      </c>
+      <c r="F240" s="32">
+        <v>13.48</v>
+      </c>
+      <c r="G240" s="32"/>
+      <c r="H240" s="75">
+        <v>17.84</v>
+      </c>
+    </row>
+    <row r="241" ht="25" customHeight="1" spans="1:8">
+      <c r="A241" s="71"/>
+      <c r="B241" s="21"/>
+      <c r="C241" s="22">
+        <v>43551</v>
+      </c>
+      <c r="D241" s="64">
+        <v>37.2335</v>
+      </c>
+      <c r="E241" s="32">
+        <v>14.64</v>
+      </c>
+      <c r="F241" s="32">
+        <v>14.65</v>
+      </c>
+      <c r="G241" s="32">
+        <v>18.7</v>
+      </c>
+      <c r="H241" s="75">
+        <v>17.96</v>
+      </c>
+    </row>
     <row r="242" ht="25" customHeight="1" spans="1:8">
-      <c r="A242" s="72" t="s">
-        <v>13</v>
-      </c>
-      <c r="B242" s="36" t="s">
+      <c r="A242" s="71"/>
+      <c r="B242" s="21"/>
+      <c r="C242" s="22"/>
+      <c r="D242" s="64"/>
+      <c r="E242" s="32"/>
+      <c r="F242" s="32"/>
+      <c r="G242" s="32"/>
+      <c r="H242" s="75"/>
+    </row>
+    <row r="243" ht="25" customHeight="1" spans="1:8">
+      <c r="A243" s="71"/>
+      <c r="B243" s="21"/>
+      <c r="C243" s="22"/>
+      <c r="D243" s="64"/>
+      <c r="E243" s="32"/>
+      <c r="F243" s="32"/>
+      <c r="G243" s="32"/>
+      <c r="H243" s="75"/>
+    </row>
+    <row r="244" ht="25" customHeight="1" spans="1:8">
+      <c r="A244" s="71"/>
+      <c r="B244" s="21"/>
+      <c r="C244" s="22"/>
+      <c r="D244" s="64"/>
+      <c r="E244" s="32"/>
+      <c r="F244" s="32"/>
+      <c r="G244" s="32"/>
+      <c r="H244" s="75"/>
+    </row>
+    <row r="245" ht="25" customHeight="1" spans="1:8">
+      <c r="A245" s="71"/>
+      <c r="B245" s="21"/>
+      <c r="C245" s="68"/>
+      <c r="D245" s="68"/>
+      <c r="E245" s="69"/>
+      <c r="F245" s="69"/>
+      <c r="G245" s="69"/>
+      <c r="H245" s="70"/>
+    </row>
+    <row r="246" ht="25" customHeight="1"/>
+    <row r="247" ht="25" customHeight="1" spans="1:8">
+      <c r="A247" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="C242" s="22">
+      <c r="B247" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="C247" s="22">
         <v>43313</v>
       </c>
-      <c r="D242" s="65">
+      <c r="D247" s="64">
         <v>102.22</v>
       </c>
-      <c r="E242" s="77">
+      <c r="E247" s="76">
         <v>11.6</v>
       </c>
-      <c r="F242" s="77">
+      <c r="F247" s="76">
         <v>21.8</v>
       </c>
-      <c r="G242" s="77">
+      <c r="G247" s="76">
         <v>16</v>
       </c>
-      <c r="H242" s="78">
+      <c r="H247" s="77">
         <v>35.2</v>
       </c>
     </row>
-    <row r="243" ht="25" customHeight="1" spans="1:8">
-      <c r="A243" s="72"/>
-      <c r="B243" s="36"/>
-      <c r="C243" s="22">
-        <v>43319</v>
-      </c>
-      <c r="D243" s="65">
-        <v>102.43</v>
-      </c>
-      <c r="E243" s="26">
-        <v>11.7</v>
-      </c>
-      <c r="F243" s="26">
-        <v>21.8</v>
-      </c>
-      <c r="G243" s="26">
-        <v>15.6</v>
-      </c>
-      <c r="H243" s="44">
-        <v>35.9</v>
-      </c>
-    </row>
-    <row r="244" ht="25" customHeight="1" spans="1:8">
-      <c r="A244" s="72"/>
-      <c r="B244" s="36"/>
-      <c r="C244" s="22">
-        <v>43321</v>
-      </c>
-      <c r="D244" s="65">
-        <v>102.93</v>
-      </c>
-      <c r="E244" s="26">
-        <v>14.7</v>
-      </c>
-      <c r="F244" s="26">
-        <v>21.9</v>
-      </c>
-      <c r="G244" s="26">
-        <v>15.8</v>
-      </c>
-      <c r="H244" s="44">
-        <v>35.9</v>
-      </c>
-    </row>
-    <row r="245" ht="25" customHeight="1" spans="1:8">
-      <c r="A245" s="72"/>
-      <c r="B245" s="36"/>
-      <c r="C245" s="22">
-        <v>43322</v>
-      </c>
-      <c r="D245" s="65">
-        <v>102.43</v>
-      </c>
-      <c r="E245" s="26">
-        <v>17.1</v>
-      </c>
-      <c r="F245" s="26">
-        <v>22.4</v>
-      </c>
-      <c r="G245" s="26">
-        <v>15.7</v>
-      </c>
-      <c r="H245" s="44">
-        <v>35.8</v>
-      </c>
-    </row>
-    <row r="246" ht="25" customHeight="1" spans="1:8">
-      <c r="A246" s="72"/>
-      <c r="B246" s="36"/>
-      <c r="C246" s="22">
-        <v>43325</v>
-      </c>
-      <c r="D246" s="65">
-        <v>101.44</v>
-      </c>
-      <c r="E246" s="26">
-        <v>15.9</v>
-      </c>
-      <c r="F246" s="26">
-        <v>21.5</v>
-      </c>
-      <c r="G246" s="26">
-        <v>17.1</v>
-      </c>
-      <c r="H246" s="44">
-        <v>34.7</v>
-      </c>
-    </row>
-    <row r="247" ht="25" customHeight="1" spans="1:8">
-      <c r="A247" s="72"/>
-      <c r="B247" s="36"/>
-      <c r="C247" s="22">
-        <v>43326</v>
-      </c>
-      <c r="D247" s="65">
-        <v>102.3</v>
-      </c>
-      <c r="E247" s="26">
-        <v>13.4</v>
-      </c>
-      <c r="F247" s="26">
-        <v>21.8</v>
-      </c>
-      <c r="G247" s="26">
-        <v>16.7</v>
-      </c>
-      <c r="H247" s="44">
-        <v>35.3</v>
-      </c>
-    </row>
     <row r="248" ht="25" customHeight="1" spans="1:8">
-      <c r="A248" s="72"/>
+      <c r="A248" s="71"/>
       <c r="B248" s="36"/>
       <c r="C248" s="22">
-        <v>43332</v>
-      </c>
-      <c r="D248" s="65">
-        <v>104.2</v>
+        <v>43319</v>
+      </c>
+      <c r="D248" s="64">
+        <v>102.43</v>
       </c>
       <c r="E248" s="26">
-        <v>16</v>
+        <v>11.7</v>
       </c>
       <c r="F248" s="26">
         <v>21.8</v>
       </c>
       <c r="G248" s="26">
-        <v>17.3</v>
+        <v>15.6</v>
       </c>
       <c r="H248" s="44">
-        <v>36.5</v>
+        <v>35.9</v>
       </c>
     </row>
     <row r="249" ht="25" customHeight="1" spans="1:8">
-      <c r="A249" s="72"/>
+      <c r="A249" s="71"/>
       <c r="B249" s="36"/>
       <c r="C249" s="22">
-        <v>43333</v>
-      </c>
-      <c r="D249" s="65">
-        <v>104.68</v>
+        <v>43321</v>
+      </c>
+      <c r="D249" s="64">
+        <v>102.93</v>
       </c>
       <c r="E249" s="26">
-        <v>18</v>
+        <v>14.7</v>
       </c>
       <c r="F249" s="26">
-        <v>22.1</v>
+        <v>21.9</v>
       </c>
       <c r="G249" s="26">
-        <v>17.6</v>
+        <v>15.8</v>
       </c>
       <c r="H249" s="44">
-        <v>36.8</v>
+        <v>35.9</v>
       </c>
     </row>
     <row r="250" ht="25" customHeight="1" spans="1:8">
-      <c r="A250" s="72"/>
+      <c r="A250" s="71"/>
       <c r="B250" s="36"/>
       <c r="C250" s="22">
-        <v>43336</v>
-      </c>
-      <c r="D250" s="65">
-        <v>104.28</v>
+        <v>43322</v>
+      </c>
+      <c r="D250" s="64">
+        <v>102.43</v>
       </c>
       <c r="E250" s="26">
-        <v>16.8</v>
+        <v>17.1</v>
       </c>
       <c r="F250" s="26">
-        <v>21.4</v>
+        <v>22.4</v>
       </c>
       <c r="G250" s="26">
-        <v>20.9</v>
+        <v>15.7</v>
       </c>
       <c r="H250" s="44">
-        <v>36.3</v>
+        <v>35.8</v>
       </c>
     </row>
     <row r="251" ht="25" customHeight="1" spans="1:8">
-      <c r="A251" s="72"/>
+      <c r="A251" s="71"/>
       <c r="B251" s="36"/>
       <c r="C251" s="22">
-        <v>43342</v>
-      </c>
-      <c r="D251" s="65">
-        <v>105.65</v>
+        <v>43325</v>
+      </c>
+      <c r="D251" s="64">
+        <v>101.44</v>
       </c>
       <c r="E251" s="26">
-        <v>16.5</v>
+        <v>15.9</v>
       </c>
       <c r="F251" s="26">
-        <v>21.4</v>
+        <v>21.5</v>
       </c>
       <c r="G251" s="26">
-        <v>20.3</v>
+        <v>17.1</v>
       </c>
       <c r="H251" s="44">
-        <v>36.9</v>
+        <v>34.7</v>
       </c>
     </row>
     <row r="252" ht="25" customHeight="1" spans="1:8">
-      <c r="A252" s="72"/>
+      <c r="A252" s="71"/>
       <c r="B252" s="36"/>
       <c r="C252" s="22">
-        <v>43348</v>
-      </c>
-      <c r="D252" s="65">
-        <v>102.34</v>
-      </c>
-      <c r="E252" s="66">
-        <v>10.6</v>
-      </c>
-      <c r="F252" s="66">
-        <v>19.3</v>
-      </c>
-      <c r="G252" s="66">
-        <v>20.4</v>
+        <v>43326</v>
+      </c>
+      <c r="D252" s="64">
+        <v>102.3</v>
+      </c>
+      <c r="E252" s="26">
+        <v>13.4</v>
+      </c>
+      <c r="F252" s="26">
+        <v>21.8</v>
+      </c>
+      <c r="G252" s="26">
+        <v>16.7</v>
       </c>
       <c r="H252" s="44">
-        <v>35.6</v>
+        <v>35.3</v>
       </c>
     </row>
     <row r="253" ht="25" customHeight="1" spans="1:8">
-      <c r="A253" s="72"/>
+      <c r="A253" s="71"/>
       <c r="B253" s="36"/>
       <c r="C253" s="22">
-        <v>43368</v>
-      </c>
-      <c r="D253" s="65">
-        <v>95.31</v>
+        <v>43332</v>
+      </c>
+      <c r="D253" s="64">
+        <v>104.2</v>
       </c>
       <c r="E253" s="26">
-        <v>3.1</v>
+        <v>16</v>
       </c>
       <c r="F253" s="26">
-        <v>14.1</v>
+        <v>21.8</v>
       </c>
       <c r="G253" s="26">
-        <v>16</v>
+        <v>17.3</v>
       </c>
       <c r="H253" s="44">
-        <v>32.9</v>
+        <v>36.5</v>
       </c>
     </row>
     <row r="254" ht="25" customHeight="1" spans="1:8">
-      <c r="A254" s="72"/>
+      <c r="A254" s="71"/>
       <c r="B254" s="36"/>
       <c r="C254" s="22">
-        <v>43383</v>
-      </c>
-      <c r="D254" s="65">
-        <v>89.78</v>
+        <v>43333</v>
+      </c>
+      <c r="D254" s="64">
+        <v>104.68</v>
       </c>
       <c r="E254" s="26">
-        <v>-4.1</v>
+        <v>18</v>
       </c>
       <c r="F254" s="26">
-        <v>9.7</v>
+        <v>22.1</v>
       </c>
       <c r="G254" s="26">
-        <v>12.3</v>
+        <v>17.6</v>
       </c>
       <c r="H254" s="44">
-        <v>29.8</v>
+        <v>36.8</v>
       </c>
     </row>
     <row r="255" ht="25" customHeight="1" spans="1:8">
-      <c r="A255" s="72"/>
+      <c r="A255" s="71"/>
       <c r="B255" s="36"/>
       <c r="C255" s="22">
-        <v>43399</v>
-      </c>
-      <c r="D255" s="28">
-        <v>86.73</v>
+        <v>43336</v>
+      </c>
+      <c r="D255" s="64">
+        <v>104.28</v>
       </c>
       <c r="E255" s="26">
-        <v>-8.6</v>
+        <v>16.8</v>
       </c>
       <c r="F255" s="26">
-        <v>7.8</v>
+        <v>21.4</v>
       </c>
       <c r="G255" s="26">
-        <v>11.2</v>
+        <v>20.9</v>
       </c>
       <c r="H255" s="44">
-        <v>28.5</v>
+        <v>36.3</v>
       </c>
     </row>
     <row r="256" ht="25" customHeight="1" spans="1:8">
-      <c r="A256" s="72"/>
+      <c r="A256" s="71"/>
       <c r="B256" s="36"/>
       <c r="C256" s="22">
-        <v>43402</v>
-      </c>
-      <c r="D256" s="28">
-        <v>89</v>
+        <v>43342</v>
+      </c>
+      <c r="D256" s="64">
+        <v>105.65</v>
       </c>
       <c r="E256" s="26">
-        <v>-6.7</v>
+        <v>16.5</v>
       </c>
       <c r="F256" s="26">
-        <v>9</v>
+        <v>21.4</v>
       </c>
       <c r="G256" s="26">
-        <v>12.4</v>
+        <v>20.3</v>
       </c>
       <c r="H256" s="44">
-        <v>28.9</v>
+        <v>36.9</v>
       </c>
     </row>
     <row r="257" ht="25" customHeight="1" spans="1:8">
-      <c r="A257" s="72"/>
+      <c r="A257" s="71"/>
       <c r="B257" s="36"/>
       <c r="C257" s="22">
-        <v>43404</v>
-      </c>
-      <c r="D257" s="31">
-        <v>90.78</v>
-      </c>
-      <c r="E257" s="26">
-        <v>-5.9</v>
-      </c>
-      <c r="F257" s="26">
-        <v>10.1</v>
-      </c>
-      <c r="G257" s="26">
-        <v>13.2</v>
+        <v>43348</v>
+      </c>
+      <c r="D257" s="64">
+        <v>102.34</v>
+      </c>
+      <c r="E257" s="65">
+        <v>10.6</v>
+      </c>
+      <c r="F257" s="65">
+        <v>19.3</v>
+      </c>
+      <c r="G257" s="65">
+        <v>20.4</v>
       </c>
       <c r="H257" s="44">
-        <v>29</v>
+        <v>35.6</v>
       </c>
     </row>
     <row r="258" ht="25" customHeight="1" spans="1:8">
-      <c r="A258" s="72"/>
+      <c r="A258" s="71"/>
       <c r="B258" s="36"/>
       <c r="C258" s="22">
-        <v>43405</v>
-      </c>
-      <c r="D258" s="31">
-        <v>91.15</v>
+        <v>43368</v>
+      </c>
+      <c r="D258" s="64">
+        <v>95.31</v>
       </c>
       <c r="E258" s="26">
-        <v>-6.2</v>
+        <v>3.1</v>
       </c>
       <c r="F258" s="26">
-        <v>9.8</v>
+        <v>14.1</v>
       </c>
       <c r="G258" s="26">
-        <v>13.4</v>
+        <v>16</v>
       </c>
       <c r="H258" s="44">
-        <v>28.9</v>
+        <v>32.9</v>
       </c>
     </row>
     <row r="259" ht="25" customHeight="1" spans="1:8">
-      <c r="A259" s="72"/>
+      <c r="A259" s="71"/>
       <c r="B259" s="36"/>
       <c r="C259" s="22">
-        <v>43410</v>
-      </c>
-      <c r="D259" s="31">
-        <v>91.31</v>
+        <v>43383</v>
+      </c>
+      <c r="D259" s="64">
+        <v>89.78</v>
       </c>
       <c r="E259" s="26">
-        <v>-6.8</v>
+        <v>-4.1</v>
       </c>
       <c r="F259" s="26">
-        <v>12.2</v>
+        <v>9.7</v>
       </c>
       <c r="G259" s="26">
-        <v>14.1</v>
+        <v>12.3</v>
       </c>
       <c r="H259" s="44">
-        <v>28.4</v>
+        <v>29.8</v>
       </c>
     </row>
     <row r="260" ht="25" customHeight="1" spans="1:8">
-      <c r="A260" s="72"/>
+      <c r="A260" s="71"/>
       <c r="B260" s="36"/>
       <c r="C260" s="22">
-        <v>43413</v>
-      </c>
-      <c r="D260" s="31">
-        <v>92.23</v>
+        <v>43399</v>
+      </c>
+      <c r="D260" s="28">
+        <v>86.73</v>
       </c>
       <c r="E260" s="26">
-        <v>-4.3</v>
+        <v>-8.6</v>
       </c>
       <c r="F260" s="26">
-        <v>13.2</v>
+        <v>7.8</v>
       </c>
       <c r="G260" s="26">
-        <v>14.3</v>
+        <v>11.2</v>
       </c>
       <c r="H260" s="44">
-        <v>29</v>
+        <v>28.5</v>
       </c>
     </row>
     <row r="261" ht="25" customHeight="1" spans="1:8">
-      <c r="A261" s="72"/>
+      <c r="A261" s="71"/>
       <c r="B261" s="36"/>
       <c r="C261" s="22">
-        <v>43430</v>
-      </c>
-      <c r="D261" s="31">
-        <v>92.21</v>
+        <v>43402</v>
+      </c>
+      <c r="D261" s="28">
+        <v>89</v>
       </c>
       <c r="E261" s="26">
-        <v>-6.2</v>
+        <v>-6.7</v>
       </c>
       <c r="F261" s="26">
-        <v>17.1</v>
+        <v>9</v>
       </c>
       <c r="G261" s="26">
-        <v>13.2</v>
+        <v>12.4</v>
       </c>
       <c r="H261" s="44">
-        <v>29</v>
+        <v>28.9</v>
       </c>
     </row>
     <row r="262" ht="25" customHeight="1" spans="1:8">
-      <c r="A262" s="72"/>
+      <c r="A262" s="71"/>
       <c r="B262" s="36"/>
       <c r="C262" s="22">
-        <v>43432</v>
+        <v>43404</v>
       </c>
       <c r="D262" s="31">
-        <v>92.68</v>
+        <v>90.78</v>
       </c>
       <c r="E262" s="26">
-        <v>-6.4</v>
+        <v>-5.9</v>
       </c>
       <c r="F262" s="26">
-        <v>17</v>
+        <v>10.1</v>
       </c>
       <c r="G262" s="26">
-        <v>13.1</v>
+        <v>13.2</v>
       </c>
       <c r="H262" s="44">
-        <v>28.8</v>
+        <v>29</v>
       </c>
     </row>
     <row r="263" ht="25" customHeight="1" spans="1:8">
-      <c r="A263" s="72"/>
+      <c r="A263" s="71"/>
       <c r="B263" s="36"/>
       <c r="C263" s="22">
-        <v>43452</v>
-      </c>
-      <c r="D263" s="65">
-        <v>94.49</v>
+        <v>43405</v>
+      </c>
+      <c r="D263" s="31">
+        <v>91.15</v>
       </c>
       <c r="E263" s="26">
-        <v>-5</v>
+        <v>-6.2</v>
       </c>
       <c r="F263" s="26">
-        <v>18.3</v>
+        <v>9.8</v>
       </c>
       <c r="G263" s="26">
-        <v>14.3</v>
+        <v>13.4</v>
       </c>
       <c r="H263" s="44">
-        <v>28.3</v>
+        <v>28.9</v>
       </c>
     </row>
     <row r="264" ht="25" customHeight="1" spans="1:8">
-      <c r="A264" s="72"/>
+      <c r="A264" s="71"/>
       <c r="B264" s="36"/>
       <c r="C264" s="22">
-        <v>43461</v>
-      </c>
-      <c r="D264" s="65">
-        <v>93.82</v>
+        <v>43410</v>
+      </c>
+      <c r="D264" s="31">
+        <v>91.31</v>
       </c>
       <c r="E264" s="26">
-        <v>-8.7</v>
+        <v>-6.8</v>
       </c>
       <c r="F264" s="26">
-        <v>19.8</v>
+        <v>12.2</v>
       </c>
       <c r="G264" s="26">
-        <v>13.3</v>
+        <v>14.1</v>
       </c>
       <c r="H264" s="44">
-        <v>27</v>
+        <v>28.4</v>
       </c>
     </row>
     <row r="265" ht="25" customHeight="1" spans="1:8">
-      <c r="A265" s="72"/>
+      <c r="A265" s="71"/>
       <c r="B265" s="36"/>
       <c r="C265" s="22">
+        <v>43413</v>
+      </c>
+      <c r="D265" s="31">
+        <v>92.23</v>
+      </c>
+      <c r="E265" s="26">
+        <v>-4.3</v>
+      </c>
+      <c r="F265" s="26">
+        <v>13.2</v>
+      </c>
+      <c r="G265" s="26">
+        <v>14.3</v>
+      </c>
+      <c r="H265" s="44">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="266" ht="25" customHeight="1" spans="1:8">
+      <c r="A266" s="71"/>
+      <c r="B266" s="36"/>
+      <c r="C266" s="22">
+        <v>43430</v>
+      </c>
+      <c r="D266" s="31">
+        <v>92.21</v>
+      </c>
+      <c r="E266" s="26">
+        <v>-6.2</v>
+      </c>
+      <c r="F266" s="26">
+        <v>17.1</v>
+      </c>
+      <c r="G266" s="26">
+        <v>13.2</v>
+      </c>
+      <c r="H266" s="44">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="267" ht="25" customHeight="1" spans="1:8">
+      <c r="A267" s="71"/>
+      <c r="B267" s="36"/>
+      <c r="C267" s="22">
+        <v>43432</v>
+      </c>
+      <c r="D267" s="31">
+        <v>92.68</v>
+      </c>
+      <c r="E267" s="26">
+        <v>-6.4</v>
+      </c>
+      <c r="F267" s="26">
+        <v>17</v>
+      </c>
+      <c r="G267" s="26">
+        <v>13.1</v>
+      </c>
+      <c r="H267" s="44">
+        <v>28.8</v>
+      </c>
+    </row>
+    <row r="268" ht="25" customHeight="1" spans="1:8">
+      <c r="A268" s="71"/>
+      <c r="B268" s="36"/>
+      <c r="C268" s="22">
+        <v>43452</v>
+      </c>
+      <c r="D268" s="64">
+        <v>94.49</v>
+      </c>
+      <c r="E268" s="26">
+        <v>-5</v>
+      </c>
+      <c r="F268" s="26">
+        <v>18.3</v>
+      </c>
+      <c r="G268" s="26">
+        <v>14.3</v>
+      </c>
+      <c r="H268" s="44">
+        <v>28.3</v>
+      </c>
+    </row>
+    <row r="269" ht="25" customHeight="1" spans="1:8">
+      <c r="A269" s="71"/>
+      <c r="B269" s="36"/>
+      <c r="C269" s="22">
+        <v>43461</v>
+      </c>
+      <c r="D269" s="64">
+        <v>93.82</v>
+      </c>
+      <c r="E269" s="26">
+        <v>-8.7</v>
+      </c>
+      <c r="F269" s="26">
+        <v>19.8</v>
+      </c>
+      <c r="G269" s="26">
+        <v>13.3</v>
+      </c>
+      <c r="H269" s="44">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="270" ht="25" customHeight="1" spans="1:8">
+      <c r="A270" s="71"/>
+      <c r="B270" s="36"/>
+      <c r="C270" s="22">
         <v>43480</v>
       </c>
-      <c r="D265" s="65">
+      <c r="D270" s="64">
         <v>94.7</v>
       </c>
-      <c r="E265" s="26">
+      <c r="E270" s="26">
         <v>-9.2</v>
       </c>
-      <c r="F265" s="26">
+      <c r="F270" s="26">
         <v>16.1</v>
       </c>
-      <c r="G265" s="26">
+      <c r="G270" s="26">
         <v>17.2</v>
       </c>
-      <c r="H265" s="44">
+      <c r="H270" s="44">
         <v>27.2</v>
       </c>
     </row>
-    <row r="266" ht="25" customHeight="1" spans="1:8">
-      <c r="A266" s="72"/>
-      <c r="B266" s="36"/>
-      <c r="C266" s="22"/>
-      <c r="D266" s="65"/>
-      <c r="E266" s="26"/>
-      <c r="F266" s="26"/>
-      <c r="G266" s="26"/>
-      <c r="H266" s="44"/>
-    </row>
-    <row r="267" ht="25" customHeight="1" spans="1:8">
-      <c r="A267" s="72"/>
-      <c r="B267" s="36"/>
-      <c r="C267" s="22"/>
-      <c r="D267" s="65"/>
-      <c r="E267" s="26"/>
-      <c r="F267" s="26"/>
-      <c r="G267" s="26"/>
-      <c r="H267" s="44"/>
-    </row>
-    <row r="268" ht="25" customHeight="1" spans="1:8">
-      <c r="A268" s="72"/>
-      <c r="B268" s="36"/>
-      <c r="C268" s="22"/>
-      <c r="D268" s="65"/>
-      <c r="E268" s="26"/>
-      <c r="F268" s="26"/>
-      <c r="G268" s="26"/>
-      <c r="H268" s="44"/>
-    </row>
-    <row r="269" ht="25" customHeight="1" spans="1:8">
-      <c r="A269" s="72"/>
-      <c r="B269" s="36"/>
-      <c r="C269" s="22"/>
-      <c r="D269" s="65"/>
-      <c r="E269" s="26"/>
-      <c r="F269" s="26"/>
-      <c r="G269" s="26"/>
-      <c r="H269" s="44"/>
-    </row>
-    <row r="270" ht="25" customHeight="1" spans="1:8">
-      <c r="A270" s="72"/>
-      <c r="B270" s="36"/>
-      <c r="C270" s="22"/>
-      <c r="D270" s="65"/>
-      <c r="E270" s="26"/>
-      <c r="F270" s="26"/>
-      <c r="G270" s="26"/>
-      <c r="H270" s="44"/>
-    </row>
     <row r="271" ht="25" customHeight="1" spans="1:8">
-      <c r="A271" s="72"/>
+      <c r="A271" s="71"/>
       <c r="B271" s="36"/>
-      <c r="C271" s="65"/>
-      <c r="D271" s="65"/>
-      <c r="E271" s="62"/>
-      <c r="F271" s="62"/>
-      <c r="G271" s="62"/>
-      <c r="H271" s="64"/>
-    </row>
-    <row r="272" ht="25" customHeight="1"/>
-    <row r="273" ht="25" customHeight="1"/>
+      <c r="C271" s="22">
+        <v>43523</v>
+      </c>
+      <c r="D271" s="64">
+        <v>93.42</v>
+      </c>
+      <c r="E271" s="26">
+        <v>-7.79</v>
+      </c>
+      <c r="F271" s="26">
+        <v>12.64</v>
+      </c>
+      <c r="G271" s="26"/>
+      <c r="H271" s="44">
+        <v>28.04</v>
+      </c>
+    </row>
+    <row r="272" ht="25" customHeight="1" spans="1:8">
+      <c r="A272" s="71"/>
+      <c r="B272" s="36"/>
+      <c r="C272" s="22">
+        <v>43550</v>
+      </c>
+      <c r="D272" s="64">
+        <v>98.81</v>
+      </c>
+      <c r="E272" s="26">
+        <v>4.41</v>
+      </c>
+      <c r="F272" s="26">
+        <v>11.03</v>
+      </c>
+      <c r="G272" s="26"/>
+      <c r="H272" s="44">
+        <v>26.17</v>
+      </c>
+    </row>
+    <row r="273" ht="25" customHeight="1" spans="1:8">
+      <c r="A273" s="71"/>
+      <c r="B273" s="36"/>
+      <c r="C273" s="22">
+        <v>43551</v>
+      </c>
+      <c r="D273" s="64">
+        <v>100.12</v>
+      </c>
+      <c r="E273" s="26">
+        <v>5.27</v>
+      </c>
+      <c r="F273" s="26">
+        <v>11.98</v>
+      </c>
+      <c r="G273" s="26">
+        <v>20.78</v>
+      </c>
+      <c r="H273" s="44">
+        <v>26</v>
+      </c>
+    </row>
     <row r="274" ht="25" customHeight="1" spans="1:8">
-      <c r="A274" s="79" t="s">
-        <v>15</v>
-      </c>
-      <c r="B274" s="80" t="s">
+      <c r="A274" s="71"/>
+      <c r="B274" s="36"/>
+      <c r="C274" s="22"/>
+      <c r="D274" s="64"/>
+      <c r="E274" s="26"/>
+      <c r="F274" s="26"/>
+      <c r="G274" s="26"/>
+      <c r="H274" s="44"/>
+    </row>
+    <row r="275" ht="25" customHeight="1" spans="1:8">
+      <c r="A275" s="71"/>
+      <c r="B275" s="36"/>
+      <c r="C275" s="22"/>
+      <c r="D275" s="64"/>
+      <c r="E275" s="26"/>
+      <c r="F275" s="26"/>
+      <c r="G275" s="26"/>
+      <c r="H275" s="44"/>
+    </row>
+    <row r="276" ht="25" customHeight="1" spans="1:8">
+      <c r="A276" s="71"/>
+      <c r="B276" s="36"/>
+      <c r="C276" s="64"/>
+      <c r="D276" s="64"/>
+      <c r="E276" s="61"/>
+      <c r="F276" s="61"/>
+      <c r="G276" s="61"/>
+      <c r="H276" s="63"/>
+    </row>
+    <row r="277" ht="25" customHeight="1"/>
+    <row r="278" ht="25" customHeight="1"/>
+    <row r="279" ht="25" customHeight="1" spans="1:8">
+      <c r="A279" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="C274" s="22">
+      <c r="B279" s="80" t="s">
+        <v>17</v>
+      </c>
+      <c r="C279" s="22">
         <v>43430</v>
       </c>
-      <c r="D274" s="81">
+      <c r="D279" s="81">
         <v>227.795</v>
       </c>
-      <c r="E274" s="82">
+      <c r="E279" s="82">
         <v>-1.7</v>
       </c>
-      <c r="F274" s="82">
+      <c r="F279" s="82">
         <v>12.1</v>
       </c>
-      <c r="G274" s="82">
+      <c r="G279" s="82">
         <v>9.5</v>
       </c>
-      <c r="H274" s="82">
+      <c r="H279" s="82">
         <v>15.4</v>
       </c>
-    </row>
-    <row r="275" ht="25" customHeight="1" spans="1:8">
-      <c r="A275" s="79"/>
-      <c r="B275" s="80"/>
-      <c r="C275" s="22">
-        <v>43432</v>
-      </c>
-      <c r="D275" s="31">
-        <v>230.33</v>
-      </c>
-      <c r="E275" s="26">
-        <v>-0.9</v>
-      </c>
-      <c r="F275" s="26">
-        <v>12.6</v>
-      </c>
-      <c r="G275" s="26">
-        <v>9.6</v>
-      </c>
-      <c r="H275" s="26">
-        <v>15.5</v>
-      </c>
-    </row>
-    <row r="276" ht="25" customHeight="1" spans="1:8">
-      <c r="A276" s="79"/>
-      <c r="B276" s="80"/>
-      <c r="C276" s="22">
-        <v>43452</v>
-      </c>
-      <c r="D276" s="65">
-        <v>235.831</v>
-      </c>
-      <c r="E276" s="26">
-        <v>0.8</v>
-      </c>
-      <c r="F276" s="26">
-        <v>14.2</v>
-      </c>
-      <c r="G276" s="26">
-        <v>11.4</v>
-      </c>
-      <c r="H276" s="26">
-        <v>15.6</v>
-      </c>
-    </row>
-    <row r="277" ht="25" customHeight="1" spans="1:8">
-      <c r="A277" s="79"/>
-      <c r="B277" s="80"/>
-      <c r="C277" s="22">
-        <v>43461</v>
-      </c>
-      <c r="D277" s="65">
-        <v>233.486</v>
-      </c>
-      <c r="E277" s="26">
-        <v>-1.6</v>
-      </c>
-      <c r="F277" s="26">
-        <v>14.6</v>
-      </c>
-      <c r="G277" s="26">
-        <v>10.5</v>
-      </c>
-      <c r="H277" s="26">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="278" ht="25" customHeight="1" spans="1:8">
-      <c r="A278" s="79"/>
-      <c r="B278" s="80"/>
-      <c r="C278" s="22">
-        <v>43480</v>
-      </c>
-      <c r="D278" s="65">
-        <v>234.424</v>
-      </c>
-      <c r="E278" s="26">
-        <v>-3</v>
-      </c>
-      <c r="F278" s="26">
-        <v>11.9</v>
-      </c>
-      <c r="G278" s="26">
-        <v>12.9</v>
-      </c>
-      <c r="H278" s="26">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="279" ht="25" customHeight="1" spans="1:8">
-      <c r="A279" s="79"/>
-      <c r="B279" s="80"/>
-      <c r="C279" s="69"/>
-      <c r="D279" s="69"/>
-      <c r="E279" s="70"/>
-      <c r="F279" s="70"/>
-      <c r="G279" s="70"/>
-      <c r="H279" s="70"/>
     </row>
     <row r="280" ht="25" customHeight="1" spans="1:8">
       <c r="A280" s="79"/>
       <c r="B280" s="80"/>
-      <c r="C280" s="69"/>
-      <c r="D280" s="69"/>
-      <c r="E280" s="70"/>
-      <c r="F280" s="70"/>
-      <c r="G280" s="70"/>
-      <c r="H280" s="70"/>
+      <c r="C280" s="22">
+        <v>43432</v>
+      </c>
+      <c r="D280" s="31">
+        <v>230.33</v>
+      </c>
+      <c r="E280" s="26">
+        <v>-0.9</v>
+      </c>
+      <c r="F280" s="26">
+        <v>12.6</v>
+      </c>
+      <c r="G280" s="26">
+        <v>9.6</v>
+      </c>
+      <c r="H280" s="26">
+        <v>15.5</v>
+      </c>
     </row>
     <row r="281" ht="25" customHeight="1" spans="1:8">
       <c r="A281" s="79"/>
       <c r="B281" s="80"/>
-      <c r="C281" s="69"/>
-      <c r="D281" s="69"/>
-      <c r="E281" s="70"/>
-      <c r="F281" s="70"/>
-      <c r="G281" s="70"/>
-      <c r="H281" s="70"/>
+      <c r="C281" s="22">
+        <v>43452</v>
+      </c>
+      <c r="D281" s="64">
+        <v>235.831</v>
+      </c>
+      <c r="E281" s="26">
+        <v>0.8</v>
+      </c>
+      <c r="F281" s="26">
+        <v>14.2</v>
+      </c>
+      <c r="G281" s="26">
+        <v>11.4</v>
+      </c>
+      <c r="H281" s="26">
+        <v>15.6</v>
+      </c>
     </row>
     <row r="282" ht="25" customHeight="1" spans="1:8">
       <c r="A282" s="79"/>
       <c r="B282" s="80"/>
-      <c r="C282" s="69"/>
-      <c r="D282" s="69"/>
-      <c r="E282" s="70"/>
-      <c r="F282" s="70"/>
-      <c r="G282" s="70"/>
-      <c r="H282" s="70"/>
-    </row>
-    <row r="283" ht="25" customHeight="1"/>
-    <row r="284" ht="25" customHeight="1"/>
-    <row r="285" ht="25" customHeight="1"/>
-    <row r="286" ht="25" customHeight="1"/>
-    <row r="287" ht="25" customHeight="1"/>
+      <c r="C282" s="22">
+        <v>43461</v>
+      </c>
+      <c r="D282" s="64">
+        <v>233.486</v>
+      </c>
+      <c r="E282" s="26">
+        <v>-1.6</v>
+      </c>
+      <c r="F282" s="26">
+        <v>14.6</v>
+      </c>
+      <c r="G282" s="26">
+        <v>10.5</v>
+      </c>
+      <c r="H282" s="26">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="283" ht="25" customHeight="1" spans="1:8">
+      <c r="A283" s="79"/>
+      <c r="B283" s="80"/>
+      <c r="C283" s="22">
+        <v>43480</v>
+      </c>
+      <c r="D283" s="64">
+        <v>234.424</v>
+      </c>
+      <c r="E283" s="26">
+        <v>-3</v>
+      </c>
+      <c r="F283" s="26">
+        <v>11.9</v>
+      </c>
+      <c r="G283" s="26">
+        <v>12.9</v>
+      </c>
+      <c r="H283" s="26">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="284" ht="25" customHeight="1" spans="1:8">
+      <c r="A284" s="79"/>
+      <c r="B284" s="80"/>
+      <c r="C284" s="22">
+        <v>43550</v>
+      </c>
+      <c r="D284" s="64">
+        <v>246.301</v>
+      </c>
+      <c r="E284" s="61">
+        <v>9.14</v>
+      </c>
+      <c r="F284" s="61">
+        <v>9.59</v>
+      </c>
+      <c r="G284" s="61"/>
+      <c r="H284" s="61">
+        <v>15.01</v>
+      </c>
+    </row>
+    <row r="285" ht="25" customHeight="1" spans="1:8">
+      <c r="A285" s="79"/>
+      <c r="B285" s="80"/>
+      <c r="C285" s="22">
+        <v>43551</v>
+      </c>
+      <c r="D285" s="64">
+        <v>245.74</v>
+      </c>
+      <c r="E285" s="61">
+        <v>7.65</v>
+      </c>
+      <c r="F285" s="61">
+        <v>10.28</v>
+      </c>
+      <c r="G285" s="61">
+        <v>13.81</v>
+      </c>
+      <c r="H285" s="61">
+        <v>15.08</v>
+      </c>
+    </row>
+    <row r="286" ht="25" customHeight="1" spans="1:8">
+      <c r="A286" s="79"/>
+      <c r="B286" s="80"/>
+      <c r="C286" s="64"/>
+      <c r="D286" s="64"/>
+      <c r="E286" s="61"/>
+      <c r="F286" s="61"/>
+      <c r="G286" s="61"/>
+      <c r="H286" s="61"/>
+    </row>
+    <row r="287" ht="25" customHeight="1" spans="1:8">
+      <c r="A287" s="79"/>
+      <c r="B287" s="80"/>
+      <c r="C287" s="64"/>
+      <c r="D287" s="64"/>
+      <c r="E287" s="61"/>
+      <c r="F287" s="61"/>
+      <c r="G287" s="61"/>
+      <c r="H287" s="61"/>
+    </row>
     <row r="288" ht="25" customHeight="1"/>
     <row r="289" ht="25" customHeight="1"/>
     <row r="290" ht="25" customHeight="1"/>
@@ -7150,11 +7400,11 @@
     <row r="341" ht="25" customHeight="1"/>
     <row r="342" ht="25" customHeight="1"/>
     <row r="343" ht="25" customHeight="1"/>
-    <row r="344" ht="15.75" customHeight="1"/>
-    <row r="345" ht="15.75" customHeight="1"/>
-    <row r="346" ht="15.75" customHeight="1"/>
-    <row r="347" ht="15.75" customHeight="1"/>
-    <row r="348" ht="15.75" customHeight="1"/>
+    <row r="344" ht="25" customHeight="1"/>
+    <row r="345" ht="25" customHeight="1"/>
+    <row r="346" ht="25" customHeight="1"/>
+    <row r="347" ht="25" customHeight="1"/>
+    <row r="348" ht="25" customHeight="1"/>
     <row r="349" ht="15.75" customHeight="1"/>
     <row r="350" ht="15.75" customHeight="1"/>
     <row r="351" ht="15.75" customHeight="1"/>
@@ -8024,6 +8274,11 @@
     <row r="1215" ht="15.75" customHeight="1"/>
     <row r="1216" ht="15.75" customHeight="1"/>
     <row r="1217" ht="15.75" customHeight="1"/>
+    <row r="1218" ht="15.75" customHeight="1"/>
+    <row r="1219" ht="15.75" customHeight="1"/>
+    <row r="1220" ht="15.75" customHeight="1"/>
+    <row r="1221" ht="15.75" customHeight="1"/>
+    <row r="1222" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="18">
     <mergeCell ref="A2:A40"/>
@@ -8032,24 +8287,25 @@
     <mergeCell ref="A107:A140"/>
     <mergeCell ref="A142:A174"/>
     <mergeCell ref="A176:A213"/>
-    <mergeCell ref="A215:A240"/>
-    <mergeCell ref="A242:A271"/>
-    <mergeCell ref="A274:A282"/>
+    <mergeCell ref="A215:A245"/>
+    <mergeCell ref="A247:A276"/>
+    <mergeCell ref="A279:A287"/>
     <mergeCell ref="B2:B40"/>
     <mergeCell ref="B42:B78"/>
     <mergeCell ref="B80:B105"/>
     <mergeCell ref="B107:B140"/>
     <mergeCell ref="B142:B174"/>
     <mergeCell ref="B176:B213"/>
-    <mergeCell ref="B215:B240"/>
-    <mergeCell ref="B242:B271"/>
-    <mergeCell ref="B274:B282"/>
+    <mergeCell ref="B215:B245"/>
+    <mergeCell ref="B247:B276"/>
+    <mergeCell ref="B279:B287"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A215:A240" r:id="rId1" display="Reliance Large Cap Fund - Direct Plan (G)"/>
-    <hyperlink ref="A242:A271" r:id="rId2" display="Canara Robeco Emerging Equities - Direct Plan (G)"/>
+    <hyperlink ref="A215:A245" r:id="rId1" display="Reliance Large Cap Fund - Direct Plan (G)"/>
+    <hyperlink ref="A247:A276" r:id="rId2" display="Canara Robeco Emerging Equities - Direct Plan (G)"/>
     <hyperlink ref="A80:A105" location="Sheet1!A204" display="=HYPERLINK(&quot;http://www.moneycontrol.com/mutual-funds/nav/reliance-top-200-fund-direct-plan/MRC940&quot;,&quot;Reliance Top 200 Fund - Direct Plan (G). New name: Reliance Large Cap Fund - Direct Plan (G)&quot;)"/>
-    <hyperlink ref="A274" r:id="rId3" display="Kotak Bluechip Fund - Direct Plan (G)"/>
+    <hyperlink ref="A279" r:id="rId3" display="Kotak Bluechip Fund - Direct Plan (G)"/>
+    <hyperlink ref="I215" r:id="rId4" display="https://www.valueresearchonline.com/funds/newsnapshot.asp?schemecode=16192"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="1" orientation="portrait"/>
@@ -8111,7 +8367,7 @@
         <v>Aditya Birla Sun Life Tax Relief 96 - Direct Plan (G)</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" s="12">
         <v>43203</v>
@@ -8197,7 +8453,7 @@
         <v>Tata India Tax Savings Fund - Direct Plan (G)</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" s="12">
         <v>43203</v>
@@ -8265,7 +8521,7 @@
         <v>Reliance Tax Saver (ELSS) Fund - Direct Plan (G)</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C14" s="12">
         <v>43203</v>
@@ -8337,7 +8593,7 @@
         <v>DSP BlackRock Tax Saver Fund - Direct Plan (G)</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C20" s="12">
         <v>43203</v>
@@ -9460,35 +9716,35 @@
     </row>
     <row r="2" ht="24.75" customHeight="1" spans="1:26">
       <c r="A2" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -9652,19 +9908,19 @@
     </row>
     <row r="7" ht="24.75" customHeight="1" spans="1:26">
       <c r="A7" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -9854,19 +10110,19 @@
     </row>
     <row r="13" ht="24.75" customHeight="1" spans="1:26">
       <c r="A13" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -10056,19 +10312,19 @@
     </row>
     <row r="19" ht="24.75" customHeight="1" spans="1:26">
       <c r="A19" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -10230,19 +10486,19 @@
     </row>
     <row r="24" ht="24.75" customHeight="1" spans="1:26">
       <c r="A24" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>

</xml_diff>